<commit_message>
directories added to filenames
</commit_message>
<xml_diff>
--- a/rozdeleni_dat.xlsx
+++ b/rozdeleni_dat.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\java\guess_the_number\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="480" yWindow="105" windowWidth="27795" windowHeight="12600"/>
   </bookViews>
@@ -36,198 +41,48 @@
     <t>17ZS_14_4_2015_03.eeg 6 2 6</t>
   </si>
   <si>
-    <t>17ZS_14_4_2015_04.eeg 7 7</t>
-  </si>
-  <si>
-    <t>17ZS_14_4_2015_05.eeg 7 4 2</t>
-  </si>
-  <si>
     <t>17ZS_14_4_2015_6.eeg 8 8</t>
   </si>
   <si>
-    <t>17ZS_14_4_2015_07.eeg 4 4</t>
-  </si>
-  <si>
     <t>17ZS_14_4_2015_8.eeg 4 4</t>
   </si>
   <si>
-    <t>17ZS_14_4_2015_9.eeg 5 5</t>
-  </si>
-  <si>
     <t>17ZS_14_4_2015_10.eeg 2 2</t>
   </si>
   <si>
-    <t>17ZS_14_4_2015_11.eeg 1 1</t>
-  </si>
-  <si>
-    <t>17ZS_14_4_2015_12.eeg 8 8</t>
-  </si>
-  <si>
-    <t>17ZS_14_4_2015_13.eeg 5 5</t>
-  </si>
-  <si>
-    <t>17ZS_14_4_2015_14.eeg 2 2</t>
-  </si>
-  <si>
-    <t>17ZS_14_4_2015_15.eeg 4 4</t>
-  </si>
-  <si>
-    <t>17ZS_14_4_2015_17.eeg 8 8</t>
-  </si>
-  <si>
-    <t>17ZS_14_4_2015_18.eeg 3 3</t>
-  </si>
-  <si>
-    <t>17ZS_14_4_2015_19.eeg 9 9</t>
-  </si>
-  <si>
-    <t>17ZS_14_4_2015_20.eeg 5 1 5</t>
-  </si>
-  <si>
-    <t>17ZS_14_4_2015_21.eeg 3 5 3</t>
-  </si>
-  <si>
-    <t>17ZS_14_4_2015_22.eeg 3 3</t>
-  </si>
-  <si>
-    <t>17ZS_14_4_2015_23.eeg 8 8</t>
-  </si>
-  <si>
-    <t>17ZS_14_4_2015_24.eeg 7 7</t>
-  </si>
-  <si>
-    <t>17ZS_14_4_2015_25.eeg 6 6</t>
-  </si>
-  <si>
     <t>blastnice_20141023_21.eeg 1 1</t>
   </si>
   <si>
-    <t>blatnice20131023_13.eeg 3 3</t>
-  </si>
-  <si>
-    <t>blatnice20141023_7.eeg 8 8</t>
-  </si>
-  <si>
     <t>blatnice20141023_8.eeg 1 1</t>
   </si>
   <si>
     <t>impedance</t>
   </si>
   <si>
-    <t>blatnice20141023_9.eeg 3 3</t>
-  </si>
-  <si>
-    <t>blatnice20141023_10.eeg 6 6</t>
-  </si>
-  <si>
-    <t>blatnice20141023_11.eeg 1 1</t>
-  </si>
-  <si>
-    <t>blatnice20141023_12.eeg 7 7</t>
-  </si>
-  <si>
-    <t>blatnice20141023_14.eeg 4 9 4</t>
-  </si>
-  <si>
-    <t>blatnice20141023_15.eeg 6 5</t>
-  </si>
-  <si>
     <t>artefakty/jetel</t>
   </si>
   <si>
-    <t>blatnice20141023_16.eeg 3 3</t>
-  </si>
-  <si>
-    <t>blatnice20141023_17.eeg 9 9</t>
-  </si>
-  <si>
     <t>Pozn:</t>
   </si>
   <si>
     <t>Blatnice - divný 1. kanál</t>
   </si>
   <si>
-    <t>blatnice20141023_18.eeg 2 5 2</t>
-  </si>
-  <si>
-    <t>blatnice20141023_19.eeg 3 3</t>
-  </si>
-  <si>
-    <t>blatnice20141023_20.eeg 2 5 2</t>
-  </si>
-  <si>
-    <t>blatnice20141023_22.eeg 3 9 7 3</t>
-  </si>
-  <si>
-    <t>blatnice20141023_23.eeg 2 6</t>
-  </si>
-  <si>
-    <t>blatnice20141023_24.eeg 1 1</t>
-  </si>
-  <si>
-    <t>DolniBela_01.eeg 7 7</t>
-  </si>
-  <si>
-    <t>DolniBela_02.eeg 7 9</t>
-  </si>
-  <si>
     <t>DolniBela_03.eeg 2 2</t>
   </si>
   <si>
-    <t>DolniBela_04.eeg 7 7</t>
-  </si>
-  <si>
     <t>DolniBela_04.eeg - kopec dolů</t>
   </si>
   <si>
-    <t>DolniBela_05.eeg 4 4</t>
-  </si>
-  <si>
-    <t>DolniBela_07.eeg 3 3</t>
-  </si>
-  <si>
-    <t>DolniBela_08.eeg 3 1 5 3</t>
-  </si>
-  <si>
-    <t>DolniBela_09.eeg 7 4</t>
-  </si>
-  <si>
-    <t>DolniBela_10.eeg 3 7 3</t>
-  </si>
-  <si>
-    <t>DolniBela_11.eeg 3 7 3</t>
-  </si>
-  <si>
-    <t>DolniBela_12.eeg 3 3</t>
-  </si>
-  <si>
     <t>DolniBela_13.eeg 3 3</t>
   </si>
   <si>
     <t>DolniBela_14.eeg 5 1</t>
   </si>
   <si>
-    <t>DolniBela_15.eeg 8 9 8</t>
-  </si>
-  <si>
-    <t>DolniBela_16.eeg 4 4</t>
-  </si>
-  <si>
-    <t>DolniBela_17.eeg 5 5</t>
-  </si>
-  <si>
     <t>DolniBela_18.eeg 4 4</t>
   </si>
   <si>
-    <t>DolniBela_19.eeg 6 6</t>
-  </si>
-  <si>
-    <t>DolniBela_20.eeg 4 4</t>
-  </si>
-  <si>
-    <t>DolniBela_06.eeg 7 4 7</t>
-  </si>
-  <si>
     <t>DolniBela_06.eeg - kopec dolů</t>
   </si>
   <si>
@@ -243,255 +98,51 @@
     <t>DolniBela_16.eeg - kopec dolů</t>
   </si>
   <si>
-    <t>Horazdovice_20140512_003.eeg 3 3</t>
-  </si>
-  <si>
     <t>Horazdovice_20141205_001.eeg 4 9 3 4</t>
   </si>
   <si>
-    <t>Horazdovice_20141204_008.eeg 5 4 2 5</t>
-  </si>
-  <si>
-    <t>Horazdovice20141204_009.eeg 7 7</t>
-  </si>
-  <si>
-    <t>Horazdovice_20141204_012.eeg 5 8 5</t>
-  </si>
-  <si>
-    <t>Horazdovice20141204_013.eeg 5 9 5</t>
-  </si>
-  <si>
-    <t>Horazdovice_20141204_014.eeg 3 7 2 1</t>
-  </si>
-  <si>
-    <t>Horazdovice_20141204_015.eeg 1 1</t>
-  </si>
-  <si>
     <t>Horazdovice_20141204_017.eeg 3 7 3</t>
   </si>
   <si>
-    <t>Horazdovice_20141204_018.eeg 1 1</t>
-  </si>
-  <si>
-    <t>Horazdovice20141204_019.eeg 7 2 5</t>
-  </si>
-  <si>
-    <t>Horazdovice20141204_021.eeg 5 5</t>
-  </si>
-  <si>
-    <t>Horazdovice20141204_022.eeg 5 5</t>
-  </si>
-  <si>
     <t>Horazdovice20141204_023.eeg 2 2</t>
   </si>
   <si>
-    <t>Horazdovice20141204_024.eeg 1 1</t>
-  </si>
-  <si>
-    <t>Horazdovice20141204_025.eeg 5 2 7 6</t>
-  </si>
-  <si>
-    <t>Horazdovice20141204_028.eeg 2 2</t>
-  </si>
-  <si>
-    <t>Horazdovice20141204_029.eeg 7 7</t>
-  </si>
-  <si>
     <t>Horazdovice20141204_030.eeg 2 2</t>
   </si>
   <si>
-    <t>Horazdovice20141204_031.eeg 5 4</t>
-  </si>
-  <si>
-    <t>Horazdovice20141204_032.eeg 7 7</t>
-  </si>
-  <si>
-    <t>Horazdovice_20141205_004.eeg 2 2</t>
-  </si>
-  <si>
     <t>Horazdovice_20141204_018.eeg - rozkmitaná</t>
   </si>
   <si>
-    <t>KarlovyVary_20150507_01.eeg 1 1</t>
-  </si>
-  <si>
-    <t>KarlovyVary_20150507_02.eeg 3 3</t>
-  </si>
-  <si>
-    <t>KarlovyVary_20150507_03.eeg 5 4 9</t>
-  </si>
-  <si>
-    <t>KarlovyVary_20150507_04.eeg 7 7</t>
-  </si>
-  <si>
-    <t>KarlovyVary_20150507_06.eeg 3 3</t>
-  </si>
-  <si>
-    <t>KarlovyVary_20150507_07.eeg 6 6</t>
-  </si>
-  <si>
-    <t>KarlovyVary_20150507_08.eeg 2 7 2</t>
-  </si>
-  <si>
-    <t>KarlovyVary_20150507_09.eeg 9 9</t>
-  </si>
-  <si>
-    <t>KarlovyVary_20150507_10.eeg 3 3</t>
-  </si>
-  <si>
-    <t>KarlovyVary_20150507_11.eeg 6 8 1</t>
-  </si>
-  <si>
-    <t>KarlovyVary_20150507_12.eeg 7 7</t>
-  </si>
-  <si>
-    <t>KarlovyVary_20150507_13.eeg 8 8</t>
-  </si>
-  <si>
-    <t>KarlovyVary_20150507_14.eeg 2 2</t>
-  </si>
-  <si>
     <t>KarlovyVary_20150507_15.eeg 4 4</t>
   </si>
   <si>
-    <t>KarlovyVary_20150507_05.eeg 6 6</t>
-  </si>
-  <si>
     <t>KarlovyVary_20150507_10.eeg - rozkmitaná</t>
   </si>
   <si>
-    <t xml:space="preserve">Masaryko002_20141124.eeg 3 3 </t>
-  </si>
-  <si>
     <t>Masaryko002_20141124.eeg - kopec dolů</t>
   </si>
   <si>
-    <t>Masarykovo001_20141124.eeg 4 4</t>
-  </si>
-  <si>
-    <t>masarykovo003_20141124.eeg 2 1 4 7</t>
-  </si>
-  <si>
-    <t>masarykovo004_20141124.eeg 3 3</t>
-  </si>
-  <si>
-    <t>masarykovo005_20141124.eeg 6 6</t>
-  </si>
-  <si>
-    <t>masarykovo006_20141124.eeg 9 9</t>
-  </si>
-  <si>
-    <t>masarykovo007_20141124.eeg 9 9</t>
-  </si>
-  <si>
-    <t>masarykovo008_20141124.eeg 1 1</t>
-  </si>
-  <si>
-    <t>masarykovo010_20141124.eeg 1 1</t>
-  </si>
-  <si>
     <t>masarykovo010_20141124.eeg - kopec dolů</t>
   </si>
   <si>
-    <t>masarykovo011_20141124.eeg 5 5</t>
-  </si>
-  <si>
-    <t>masarykovo012_20141124.eeg 9 9</t>
-  </si>
-  <si>
-    <t>masarykovo013_20141124.eeg 8 8</t>
-  </si>
-  <si>
-    <t>masarykovo014_20141124.eeg 2 7 8</t>
-  </si>
-  <si>
-    <t>masarykovo015_20141124.eeg 3 9</t>
-  </si>
-  <si>
-    <t>masarykovo016_20141124.eeg 4 4</t>
-  </si>
-  <si>
-    <t>masarykovo017_20141124.eeg 2 2</t>
-  </si>
-  <si>
-    <t>masarykovo018_20141124.eeg 6 6</t>
-  </si>
-  <si>
-    <t>masarykovo019_20141124.eeg 7 7</t>
-  </si>
-  <si>
     <t>masarykovo019_20141124.eeg - kopec dolů, GND 8</t>
   </si>
   <si>
-    <t>masarykovo020_20141124.eeg 4 4</t>
-  </si>
-  <si>
     <t>masarykovo021_20141124.eeg 8 8</t>
   </si>
   <si>
-    <t>SPSD_3_2_2015_01.eeg 8 8</t>
-  </si>
-  <si>
-    <t>SPSD_3_2_2015_02.eeg 4 3</t>
-  </si>
-  <si>
-    <t>SPSD_3_2_2015_03.eeg 7 6 5</t>
-  </si>
-  <si>
     <t>SPSD_3_2_2015_03.eeg - neuhádnuto</t>
   </si>
   <si>
     <t>SPSD_3_2_2015_04.eeg 1 4 1</t>
   </si>
   <si>
-    <t>SPSD_3_2_2015_05.eeg 4 6 4</t>
-  </si>
-  <si>
-    <t>SPSD_3_2_2015_06.eeg 8 8</t>
-  </si>
-  <si>
-    <t>SPSD_3_2_2015_07.eeg 5 5</t>
-  </si>
-  <si>
-    <t>SPSD_3_2_2015_08.eeg 6 9 1</t>
-  </si>
-  <si>
-    <t>SPSD_3_2_2015_09.eeg 7 7</t>
-  </si>
-  <si>
     <t>SPSD_3_2_2015_10.eeg 3 7 3</t>
   </si>
   <si>
-    <t>Stankov_26_01_2015_01.eeg 1 1</t>
-  </si>
-  <si>
-    <t>Stankov_26_01_2015_02.eeg 2 2</t>
-  </si>
-  <si>
-    <t>Strankov_26_01_2015_03.eeg 5 4 5</t>
-  </si>
-  <si>
-    <t>Stankov_26_01_2015_04.eeg 7 7</t>
-  </si>
-  <si>
-    <t>Stankov_26_01_2015_05.eeg 1 1</t>
-  </si>
-  <si>
-    <t>Stankov_26_01_2015_06.eeg 2 2</t>
-  </si>
-  <si>
-    <t>Stankov_26_1_2015_07.eeg 5 5</t>
-  </si>
-  <si>
     <t>Stankov_26_01_2015_08.eeg 5 5</t>
   </si>
   <si>
-    <t>Stankov_26_01_2015_09.eeg 3 3</t>
-  </si>
-  <si>
-    <t>Stankov_26_1_2015_10.eeg 6 6</t>
-  </si>
-  <si>
     <t>Stankov_26_1_2015_10.eeg - kopec dolů</t>
   </si>
   <si>
@@ -501,66 +152,30 @@
     <t>Stankov_26_1_2015_12.eeg 5 9 6 3</t>
   </si>
   <si>
-    <t>Stankov_26_1_2015_13.eeg 5 5</t>
-  </si>
-  <si>
-    <t>Stankov_26_1_2015_14.eeg 5 6 7</t>
-  </si>
-  <si>
     <t>Stankov_26_01_2015_15.eeg 4 4</t>
   </si>
   <si>
-    <t>Stankov_26_01_2015_16.eeg 7 7</t>
-  </si>
-  <si>
-    <t>Stankov_26_1_2015_17.eeg 8 5 1 8</t>
-  </si>
-  <si>
     <t>Stankov_26_1_2015_18.eeg 8 5 1 8</t>
   </si>
   <si>
-    <t>Stankov_26_1_2015_19.eeg 7 7</t>
-  </si>
-  <si>
-    <t>Stankov_26_1_2015_20.eeg 2 4 8 1</t>
-  </si>
-  <si>
     <t>Stankov_26_01_2015_21.eeg 6 6</t>
   </si>
   <si>
-    <t>Stankov_26_01_2015_22.eeg 7 7</t>
-  </si>
-  <si>
     <t>Stankov_26_01_2015_22.eeg - rozkmitaná</t>
   </si>
   <si>
-    <t>Stankov_26_1_2015_23.eeg 3 3</t>
-  </si>
-  <si>
     <t>Stankov_26_1_2015_23.eeg -  rozkmitaná</t>
   </si>
   <si>
     <t>Stankov_26_1_2015_24.eeg 5 5</t>
   </si>
   <si>
-    <t>Stankov_26_1_2015_25.eeg 7 5</t>
-  </si>
-  <si>
-    <t>Stankov_26_1_20145_27.eeg 4 4</t>
-  </si>
-  <si>
-    <t>Stankov_26_1_2015_28.eeg 6 2</t>
-  </si>
-  <si>
     <t>Stankov_26_1_2015_29.eeg 9 1</t>
   </si>
   <si>
     <t>pd_strasice_7_1_2015_01.eeg 3 3</t>
   </si>
   <si>
-    <t>PD_Strasice_7_1_2015_02.eeg 5 5</t>
-  </si>
-  <si>
     <t>PD_Strasice_7_1_2015_02.eeg - rozkmitaná</t>
   </si>
   <si>
@@ -570,153 +185,39 @@
     <t>PD_Strasice_7_1_2015_04.eeg 5 5</t>
   </si>
   <si>
-    <t>PD_Strasice_7_1_2015_05.eeg 1 1</t>
-  </si>
-  <si>
-    <t>PD_Strasice_7_1_2015_06.eeg 7 4 7</t>
-  </si>
-  <si>
-    <t>PD_Strasice_7_1_2015_07.eeg 3 3</t>
-  </si>
-  <si>
-    <t>PD_Strasice_7_1_2015_08.eeg 2 2</t>
-  </si>
-  <si>
-    <t>PD_Strasice_7_1_2015_09.eeg 3 3</t>
-  </si>
-  <si>
-    <t>PD_Strasice_7_1_2015_10.eeg 8 8</t>
-  </si>
-  <si>
-    <t>PD_Strasice_7_1_2015_11.eeg 4 4</t>
-  </si>
-  <si>
-    <t>PD_Strasice_7_1_2015_12.eeg 2 2</t>
-  </si>
-  <si>
-    <t>PD_Strasice_7_1_2015_13.eeg 2 2</t>
-  </si>
-  <si>
-    <t>PD_Strasice_7_1_2015_14.eeg 8 8</t>
-  </si>
-  <si>
     <t>PD_Strasice_7_2015_15.eeg 8 8</t>
   </si>
   <si>
     <t>Strasice_4_2_2015_01.eeg 4 2 9 1</t>
   </si>
   <si>
-    <t>Strasice_4_2_2015_02.eeg 1 1</t>
-  </si>
-  <si>
-    <t>Strasice_4_2_2015_03.eeg 2 2</t>
-  </si>
-  <si>
-    <t>Strasice_4_2_2015_04.eeg 2 2</t>
-  </si>
-  <si>
     <t>Strasice_4_2_2015_05.eeg 2 1 8</t>
   </si>
   <si>
-    <t>Strasice_4_2_2015_07.eeg 7 7</t>
-  </si>
-  <si>
-    <t>Strasice_4_2_2015_08.eeg 3 7</t>
-  </si>
-  <si>
-    <t>Strasice_4_2_2015_09.eeg 6 4 6</t>
-  </si>
-  <si>
     <t>Strasice_4_2_2015_10.eeg 6 4 6</t>
   </si>
   <si>
     <t>Strasice_4_2_2015_10.eeg  - stejný popis jako u 09</t>
   </si>
   <si>
-    <t>Strasice_4_2_2015_11.eeg 3 3</t>
-  </si>
-  <si>
-    <t>Strasice_4_2_2015_12.eeg 3 3</t>
-  </si>
-  <si>
-    <t>Strasice_4_2_2015_13.eeg 5 5</t>
-  </si>
-  <si>
-    <t>Strasice_4_2_2015_14.eeg 6 1 6</t>
-  </si>
-  <si>
     <t>Strasice_4_2_2015_15.eeg 3 3</t>
   </si>
   <si>
     <t>Strasice_4_2_2015_16.eeg 2 3 2</t>
   </si>
   <si>
-    <t>Strasice_4_2_2015_17.eeg 9 9</t>
-  </si>
-  <si>
-    <t>Strasice_4_2_2015_18.eeg 6 6</t>
-  </si>
-  <si>
-    <t>Strasice_4_2_2015_19.eeg 2 1 2</t>
-  </si>
-  <si>
-    <t>Strasice_4_2_2015_20.eeg 5 2 5</t>
-  </si>
-  <si>
-    <t>Strasice_4_2_2015_21.eeg 2 1 2</t>
-  </si>
-  <si>
-    <t>Strasice_4_2_2015_22.eeg 8 8</t>
-  </si>
-  <si>
-    <t>Tachov_26_3_2015_01.eeg 7 7</t>
-  </si>
-  <si>
-    <t>Tachov_26_3_2015_02.eeg 3 3</t>
-  </si>
-  <si>
     <t>Tachov_26_3_2015_02.eeg - kopec dolů</t>
   </si>
   <si>
-    <t>Tachov_26_3_2015_03.eeg 9 9</t>
-  </si>
-  <si>
-    <t>Tachov_26_3_2015_04.eeg 4 6 2</t>
-  </si>
-  <si>
     <t>Tachov_26_3_2015_05.eeg 2 1 9 6</t>
   </si>
   <si>
-    <t>Tachov_26_3_2015_06.eeg 7 7</t>
-  </si>
-  <si>
-    <t>Tachov_26_3_2015_07.eeg 5 6 2</t>
-  </si>
-  <si>
-    <t>Tachov_26_3_2015_08.eeg 7 7</t>
-  </si>
-  <si>
-    <t>Tachov_26_3_2015_09.eeg 8 5 8</t>
-  </si>
-  <si>
-    <t>Tachov_26_3_2015_10.eeg 2 2</t>
-  </si>
-  <si>
     <t>Tachov_26_3_2015_11.eeg 2 8 1</t>
   </si>
   <si>
-    <t>ZSBolevecka_26_5_2015_01.eeg 9 9</t>
-  </si>
-  <si>
     <t>ZSBolevecka_26_5_2015_02.eeg 5 5</t>
   </si>
   <si>
-    <t>ZSBolevecka_26_5_2015_03.eeg 3 3</t>
-  </si>
-  <si>
-    <t>ZSBolevecka_26_5_2015_04.eeg 9 9</t>
-  </si>
-  <si>
     <t>ZSBolevecka_26_5_2015_05.eeg 8 8</t>
   </si>
   <si>
@@ -726,12 +227,6 @@
     <t>BoleveckaZS_26_5_2015_07.eeg 3 9</t>
   </si>
   <si>
-    <t>ZSBolevecka_26_5_2015_08.eeg 3 9</t>
-  </si>
-  <si>
-    <t>BoleveckaZS_26_5_2015_09.eeg 7 9</t>
-  </si>
-  <si>
     <t>ZSBolevec_26_5_2015_10.eeg 6 4 9 7</t>
   </si>
   <si>
@@ -744,12 +239,6 @@
     <t>BoleveckaZS_26_5_2015_13.eeg 7 7</t>
   </si>
   <si>
-    <t>ZSBolevecka_26_05_2015_14.eeg 6 6</t>
-  </si>
-  <si>
-    <t>Horazdovice_26_5_2015_15.eeg 7 7</t>
-  </si>
-  <si>
     <t>Horazdovice_26_5_2015_15.eeg - rozkmitaná</t>
   </si>
   <si>
@@ -762,60 +251,15 @@
     <t>BoleveckaZS_26_5_2015_19.eeg 7 4</t>
   </si>
   <si>
-    <t>BoleveckaZS_26_5_2015_20.eeg 3 3</t>
-  </si>
-  <si>
-    <t>BoleveckaZS_26_5_2015_21.eeg 4 4</t>
-  </si>
-  <si>
-    <t>Tachov_14_5_2015_01.eeg 7 7</t>
-  </si>
-  <si>
-    <t>Tachov_14_5_2015_02.eeg 9 9</t>
-  </si>
-  <si>
     <t>Tachov_14_05_2015_03.eeg 2 5 3</t>
   </si>
   <si>
-    <t>Tachov_14_5_2015_04.eeg 6 3 5 6</t>
-  </si>
-  <si>
-    <t>Tachov_14_05_2015_05.eeg 9 6 8 1 4</t>
-  </si>
-  <si>
-    <t>Tachov_14_5_2015_06.eeg 3 3</t>
-  </si>
-  <si>
     <t>Tachov_14_5_2015_06.eeg - rozkmitaná</t>
   </si>
   <si>
-    <t>Tachov_14_5_2015_07.eeg 3 6 1 5</t>
-  </si>
-  <si>
-    <t>Tachov_14_5_2015_08.eeg 5 5</t>
-  </si>
-  <si>
-    <t>Tachov_14_5_2015_09.eeg 4 9 7 1</t>
-  </si>
-  <si>
-    <t>Tachov_14_05_2015_10.eeg 5 5</t>
-  </si>
-  <si>
-    <t>Tachov_14_5_2015_11.eeg 2 4 5</t>
-  </si>
-  <si>
     <t>Tachov_14_5_2015_12.eeg 9 9</t>
   </si>
   <si>
-    <t>Tachov_14_5_2015_13.eeg 8 5 8</t>
-  </si>
-  <si>
-    <t>Tachov_14_05_2015_15.eeg 8 8</t>
-  </si>
-  <si>
-    <t>Tachov_14_5_2015_16.eeg 6 6</t>
-  </si>
-  <si>
     <t>Tachov_14_5_2015_16.eeg mírně rozkmitaná</t>
   </si>
   <si>
@@ -831,10 +275,571 @@
     <t>Tachov_14_5_2015_19.eeg - stejný popis jako u 18</t>
   </si>
   <si>
-    <t>Tachov_14_5_2015_20.eeg 6 5 6</t>
-  </si>
-  <si>
-    <t>Tachov_14_5_2015_21.eeg 9 9</t>
+    <t>17ZS/17ZS_14_4_2015_05.eeg 7 4 2</t>
+  </si>
+  <si>
+    <t>17ZS/17ZS_14_4_2015_20.eeg 5 1 5</t>
+  </si>
+  <si>
+    <t>17ZS/17ZS_14_4_2015_25.eeg 6 6</t>
+  </si>
+  <si>
+    <t>Blatnice/blatnice20131023_13.eeg 3 3</t>
+  </si>
+  <si>
+    <t>Blatnice/blatnice20141023_9.eeg 3 3</t>
+  </si>
+  <si>
+    <t>Blatnice/blatnice20141023_14.eeg 4 9 4</t>
+  </si>
+  <si>
+    <t>Blatnice/blatnice20141023_15.eeg 6 5</t>
+  </si>
+  <si>
+    <t>Blatnice/blatnice20141023_16.eeg 3 3</t>
+  </si>
+  <si>
+    <t>Blatnice/blatnice20141023_18.eeg 2 5 2</t>
+  </si>
+  <si>
+    <t>Blatnice/blatnice20141023_19.eeg 3 3</t>
+  </si>
+  <si>
+    <t>Blatnice/blatnice20141023_22.eeg 3 9 7 3</t>
+  </si>
+  <si>
+    <t>Blatnice/blatnice20141023_23.eeg 2 6</t>
+  </si>
+  <si>
+    <t>DolniBela/DolniBela_02.eeg 7 9</t>
+  </si>
+  <si>
+    <t>DolniBela/DolniBela_07.eeg 3 3</t>
+  </si>
+  <si>
+    <t>DolniBela/DolniBela_08.eeg 3 1 5 3</t>
+  </si>
+  <si>
+    <t>DolniBela/DolniBela_09.eeg 7 4</t>
+  </si>
+  <si>
+    <t>DolniBela/DolniBela_10.eeg 3 7 3</t>
+  </si>
+  <si>
+    <t>DolniBela/DolniBela_11.eeg 3 7 3</t>
+  </si>
+  <si>
+    <t>DolniBela/DolniBela_15.eeg 8 9 8</t>
+  </si>
+  <si>
+    <t>DolniBela/DolniBela_19.eeg 6 6</t>
+  </si>
+  <si>
+    <t>Horazdovice/Horazdovice_20141204_008.eeg 5 4 2 5</t>
+  </si>
+  <si>
+    <t>Horazdovice/Horazdovice20141204_009.eeg 7 7</t>
+  </si>
+  <si>
+    <t>Horazdovice/Horazdovice_20141205_004.eeg 2 2</t>
+  </si>
+  <si>
+    <t>Horazdovice/Horazdovice_20141204_012.eeg 5 8 5</t>
+  </si>
+  <si>
+    <t>Horazdovice/Horazdovice_20141204_014.eeg 3 7 2 1</t>
+  </si>
+  <si>
+    <t>Horazdovice/Horazdovice20141204_022.eeg 5 5</t>
+  </si>
+  <si>
+    <t>Horazdovice/Horazdovice20141204_024.eeg 1 1</t>
+  </si>
+  <si>
+    <t>Horazdovice/Horazdovice20141204_025.eeg 5 2 7 6</t>
+  </si>
+  <si>
+    <t>Horazdovice/Horazdovice20141204_028.eeg 2 2</t>
+  </si>
+  <si>
+    <t>Horazdovice/Horazdovice20141204_031.eeg 5 4</t>
+  </si>
+  <si>
+    <t>KVary/KarlovyVary_20150507_03.eeg 5 4 9</t>
+  </si>
+  <si>
+    <t>KVary/KarlovyVary_20150507_04.eeg 7 7</t>
+  </si>
+  <si>
+    <t>KVary/KarlovyVary_20150507_05.eeg 6 6</t>
+  </si>
+  <si>
+    <t>KVary/KarlovyVary_20150507_08.eeg 2 7 2</t>
+  </si>
+  <si>
+    <t>KVary/KarlovyVary_20150507_11.eeg 6 8 1</t>
+  </si>
+  <si>
+    <t>Masarykovo/masarykovo003_20141124.eeg 2 1 4 7</t>
+  </si>
+  <si>
+    <t>Masarykovo/masarykovo005_20141124.eeg 6 6</t>
+  </si>
+  <si>
+    <t>Masarykovo/masarykovo011_20141124.eeg 5 5</t>
+  </si>
+  <si>
+    <t>Masarykovo/masarykovo014_20141124.eeg 2 7 8</t>
+  </si>
+  <si>
+    <t>Masarykovo/masarykovo015_20141124.eeg 3 9</t>
+  </si>
+  <si>
+    <t>Masarykovo/masarykovo017_20141124.eeg 2 2</t>
+  </si>
+  <si>
+    <t>Masarykovo/masarykovo018_20141124.eeg 6 6</t>
+  </si>
+  <si>
+    <t>Masarykovo/masarykovo020_20141124.eeg 4 4</t>
+  </si>
+  <si>
+    <t>SPSD/SPSD_3_2_2015_02.eeg 4 3</t>
+  </si>
+  <si>
+    <t>SPSD/SPSD_3_2_2015_05.eeg 4 6 4</t>
+  </si>
+  <si>
+    <t>SPSD/SPSD_3_2_2015_08.eeg 6 9 1</t>
+  </si>
+  <si>
+    <t>Stankov/Strankov_26_01_2015_03.eeg 5 4 5</t>
+  </si>
+  <si>
+    <t>Stankov/Stankov_26_01_2015_04.eeg 7 7</t>
+  </si>
+  <si>
+    <t>Stankov/Stankov_26_01_2015_05.eeg 1 1</t>
+  </si>
+  <si>
+    <t>Stankov/Stankov_26_01_2015_06.eeg 2 2</t>
+  </si>
+  <si>
+    <t>Stankov/Stankov_26_1_2015_13.eeg 5 5</t>
+  </si>
+  <si>
+    <t>Stankov/Stankov_26_1_2015_14.eeg 5 6 7</t>
+  </si>
+  <si>
+    <t>Stankov/Stankov_26_1_2015_17.eeg 8 5 1 8</t>
+  </si>
+  <si>
+    <t>Stankov/Stankov_26_1_2015_19.eeg 7 7</t>
+  </si>
+  <si>
+    <t>Stankov/Stankov_26_1_2015_20.eeg 2 4 8 1</t>
+  </si>
+  <si>
+    <t>Stankov/Stankov_26_1_2015_25.eeg 7 5</t>
+  </si>
+  <si>
+    <t>Stankov/Stankov_26_1_2015_28.eeg 6 2</t>
+  </si>
+  <si>
+    <t>Strasice/PD_Strasice_7_1_2015_07.eeg 3 3</t>
+  </si>
+  <si>
+    <t>Strasice/PD_Strasice_7_1_2015_09.eeg 3 3</t>
+  </si>
+  <si>
+    <t>Strasice/PD_Strasice_7_1_2015_10.eeg 8 8</t>
+  </si>
+  <si>
+    <t>Strasice/PD_Strasice_7_1_2015_12.eeg 2 2</t>
+  </si>
+  <si>
+    <t>Strasice2/Strasice_4_2_2015_02.eeg 1 1</t>
+  </si>
+  <si>
+    <t>Strasice2/Strasice_4_2_2015_07.eeg 7 7</t>
+  </si>
+  <si>
+    <t>Strasice2/Strasice_4_2_2015_08.eeg 3 7</t>
+  </si>
+  <si>
+    <t>Strasice2/Strasice_4_2_2015_11.eeg 3 3</t>
+  </si>
+  <si>
+    <t>Strasice2/Strasice_4_2_2015_12.eeg 3 3</t>
+  </si>
+  <si>
+    <t>Strasice2/Strasice_4_2_2015_17.eeg 9 9</t>
+  </si>
+  <si>
+    <t>Strasice2/Strasice_4_2_2015_19.eeg 2 1 2</t>
+  </si>
+  <si>
+    <t>Strasice2/Strasice_4_2_2015_20.eeg 5 2 5</t>
+  </si>
+  <si>
+    <t>Strasice2/Strasice_4_2_2015_21.eeg 2 1 2</t>
+  </si>
+  <si>
+    <t>Tachov/Tachov_26_3_2015_04.eeg 4 6 2</t>
+  </si>
+  <si>
+    <t>Tachov/Tachov_26_3_2015_06.eeg 7 7</t>
+  </si>
+  <si>
+    <t>Tachov/Tachov_26_3_2015_07.eeg 5 6 2</t>
+  </si>
+  <si>
+    <t>ZSBolevecka/ZSBolevecka_26_5_2015_04.eeg 9 9</t>
+  </si>
+  <si>
+    <t>ZSBolevecka/ZSBolevecka_26_5_2015_08.eeg 3 9</t>
+  </si>
+  <si>
+    <t>ZSBolevecka/BoleveckaZS_26_5_2015_09.eeg 7 9</t>
+  </si>
+  <si>
+    <t>Tachov2/Tachov_14_5_2015_01.eeg 7 7</t>
+  </si>
+  <si>
+    <t>Tachov2/Tachov_14_5_2015_02.eeg 9 9</t>
+  </si>
+  <si>
+    <t>Tachov2/Tachov_14_05_2015_05.eeg 9 6 8 1 4</t>
+  </si>
+  <si>
+    <t>Tachov2/Tachov_14_5_2015_07.eeg 3 6 1 5</t>
+  </si>
+  <si>
+    <t>Tachov2/Tachov_14_5_2015_09.eeg 4 9 7 1</t>
+  </si>
+  <si>
+    <t>Tachov2/Tachov_14_5_2015_11.eeg 2 4 5</t>
+  </si>
+  <si>
+    <t>17ZS/17ZS_14_4_2015_04.eeg 7 7</t>
+  </si>
+  <si>
+    <t>17ZS/17ZS_14_4_2015_07.eeg 4 4</t>
+  </si>
+  <si>
+    <t>17ZS/17ZS_14_4_2015_9.eeg 5 5</t>
+  </si>
+  <si>
+    <t>17ZS/17ZS_14_4_2015_11.eeg 1 1</t>
+  </si>
+  <si>
+    <t>17ZS/17ZS_14_4_2015_12.eeg 8 8</t>
+  </si>
+  <si>
+    <t>17ZS/17ZS_14_4_2015_15.eeg 4 4</t>
+  </si>
+  <si>
+    <t>17ZS/17ZS_14_4_2015_17.eeg 8 8</t>
+  </si>
+  <si>
+    <t>17ZS/17ZS_14_4_2015_18.eeg 3 3</t>
+  </si>
+  <si>
+    <t>17ZS/17ZS_14_4_2015_19.eeg 9 9</t>
+  </si>
+  <si>
+    <t>17ZS/17ZS_14_4_2015_21.eeg 3 5 3</t>
+  </si>
+  <si>
+    <t>17ZS/17ZS_14_4_2015_22.eeg 3 3</t>
+  </si>
+  <si>
+    <t>17ZS/17ZS_14_4_2015_23.eeg 8 8</t>
+  </si>
+  <si>
+    <t>17ZS/17ZS_14_4_2015_24.eeg 7 7</t>
+  </si>
+  <si>
+    <t>Blatnice/blatnice20141023_7.eeg 8 8</t>
+  </si>
+  <si>
+    <t>Blatnice/blatnice20141023_10.eeg 6 6</t>
+  </si>
+  <si>
+    <t>Blatnice/blatnice20141023_11.eeg 1 1</t>
+  </si>
+  <si>
+    <t>Blatnice/blatnice20141023_12.eeg 7 7</t>
+  </si>
+  <si>
+    <t>Blatnice/blatnice20141023_17.eeg 9 9</t>
+  </si>
+  <si>
+    <t>DolniBela/DolniBela_04.eeg 7 7</t>
+  </si>
+  <si>
+    <t>DolniBela/DolniBela_05.eeg 4 4</t>
+  </si>
+  <si>
+    <t>DolniBela/DolniBela_06.eeg 7 4 7</t>
+  </si>
+  <si>
+    <t>DolniBela/DolniBela_12.eeg 3 3</t>
+  </si>
+  <si>
+    <t>DolniBela/DolniBela_16.eeg 4 4</t>
+  </si>
+  <si>
+    <t>Horazdovice/Horazdovice20141204_013.eeg 5 9 5</t>
+  </si>
+  <si>
+    <t>Horazdovice/Horazdovice_20141204_015.eeg 1 1</t>
+  </si>
+  <si>
+    <t>Horazdovice/Horazdovice_20141204_018.eeg 1 1</t>
+  </si>
+  <si>
+    <t>Horazdovice/Horazdovice20141204_019.eeg 7 2 5</t>
+  </si>
+  <si>
+    <t>Horazdovice/Horazdovice20141204_021.eeg 5 5</t>
+  </si>
+  <si>
+    <t>Horazdovice/Horazdovice20141204_029.eeg 7 7</t>
+  </si>
+  <si>
+    <t>Horazdovice/Horazdovice20141204_032.eeg 7 7</t>
+  </si>
+  <si>
+    <t>KVary/KarlovyVary_20150507_01.eeg 1 1</t>
+  </si>
+  <si>
+    <t>KVary/KarlovyVary_20150507_02.eeg 3 3</t>
+  </si>
+  <si>
+    <t>KVary/KarlovyVary_20150507_06.eeg 3 3</t>
+  </si>
+  <si>
+    <t>KVary/KarlovyVary_20150507_07.eeg 6 6</t>
+  </si>
+  <si>
+    <t>KVary/KarlovyVary_20150507_10.eeg 3 3</t>
+  </si>
+  <si>
+    <t>KVary/KarlovyVary_20150507_12.eeg 7 7</t>
+  </si>
+  <si>
+    <t>KVary/KarlovyVary_20150507_13.eeg 8 8</t>
+  </si>
+  <si>
+    <t>KVary/KarlovyVary_20150507_14.eeg 2 2</t>
+  </si>
+  <si>
+    <t>Masarykovo/Masaryko002_20141124.eeg 3 3</t>
+  </si>
+  <si>
+    <t>Masarykovo/Masarykovo001_20141124.eeg 4 4</t>
+  </si>
+  <si>
+    <t>Masarykovo/masarykovo004_20141124.eeg 3 3</t>
+  </si>
+  <si>
+    <t>Masarykovo/masarykovo006_20141124.eeg 9 9</t>
+  </si>
+  <si>
+    <t>Masarykovo/masarykovo010_20141124.eeg 1 1</t>
+  </si>
+  <si>
+    <t>Masarykovo/masarykovo012_20141124.eeg 9 9</t>
+  </si>
+  <si>
+    <t>Masarykovo/masarykovo013_20141124.eeg 8 8</t>
+  </si>
+  <si>
+    <t>Masarykovo/masarykovo016_20141124.eeg 4 4</t>
+  </si>
+  <si>
+    <t>Masarykovo/masarykovo019_20141124.eeg 7 7</t>
+  </si>
+  <si>
+    <t>SPSD/SPSD_3_2_2015_01.eeg 8 8</t>
+  </si>
+  <si>
+    <t>SPSD/SPSD_3_2_2015_03.eeg 7 6 5</t>
+  </si>
+  <si>
+    <t>SPSD/SPSD_3_2_2015_06.eeg 8 8</t>
+  </si>
+  <si>
+    <t>SPSD/SPSD_3_2_2015_07.eeg 5 5</t>
+  </si>
+  <si>
+    <t>SPSD/SPSD_3_2_2015_09.eeg 7 7</t>
+  </si>
+  <si>
+    <t>Stankov/Stankov_26_01_2015_01.eeg 1 1</t>
+  </si>
+  <si>
+    <t>Stankov/Stankov_26_01_2015_02.eeg 2 2</t>
+  </si>
+  <si>
+    <t>Stankov/Stankov_26_1_2015_07.eeg 5 5</t>
+  </si>
+  <si>
+    <t>Stankov/Stankov_26_01_2015_09.eeg 3 3</t>
+  </si>
+  <si>
+    <t>Stankov/Stankov_26_1_2015_10.eeg 6 6</t>
+  </si>
+  <si>
+    <t>Stankov/Stankov_26_01_2015_16.eeg 7 7</t>
+  </si>
+  <si>
+    <t>Stankov/Stankov_26_01_2015_22.eeg 7 7</t>
+  </si>
+  <si>
+    <t>Stankov/Stankov_26_1_2015_23.eeg 3 3</t>
+  </si>
+  <si>
+    <t>Strasice/PD_Strasice_7_1_2015_05.eeg 1 1</t>
+  </si>
+  <si>
+    <t>Strasice/PD_Strasice_7_1_2015_06.eeg 7 4 7</t>
+  </si>
+  <si>
+    <t>Strasice/PD_Strasice_7_1_2015_08.eeg 2 2</t>
+  </si>
+  <si>
+    <t>Strasice/PD_Strasice_7_1_2015_11.eeg 4 4</t>
+  </si>
+  <si>
+    <t>Strasice/PD_Strasice_7_1_2015_13.eeg 2 2</t>
+  </si>
+  <si>
+    <t>Strasice/PD_Strasice_7_1_2015_14.eeg 8 8</t>
+  </si>
+  <si>
+    <t>Strasice2/Strasice_4_2_2015_03.eeg 2 2</t>
+  </si>
+  <si>
+    <t>Strasice2/Strasice_4_2_2015_04.eeg 2 2</t>
+  </si>
+  <si>
+    <t>Strasice2/Strasice_4_2_2015_09.eeg 6 4 6</t>
+  </si>
+  <si>
+    <t>Strasice2/Strasice_4_2_2015_13.eeg 5 5</t>
+  </si>
+  <si>
+    <t>Strasice2/Strasice_4_2_2015_14.eeg 6 1 6</t>
+  </si>
+  <si>
+    <t>Strasice2/Strasice_4_2_2015_18.eeg 6 6</t>
+  </si>
+  <si>
+    <t>Strasice2/Strasice_4_2_2015_22.eeg 8 8</t>
+  </si>
+  <si>
+    <t>Tachov/Tachov_26_3_2015_01.eeg 7 7</t>
+  </si>
+  <si>
+    <t>Tachov/Tachov_26_3_2015_02.eeg 3 3</t>
+  </si>
+  <si>
+    <t>Tachov/Tachov_26_3_2015_03.eeg 9 9</t>
+  </si>
+  <si>
+    <t>Tachov/Tachov_26_3_2015_08.eeg 7 7</t>
+  </si>
+  <si>
+    <t>Tachov/Tachov_26_3_2015_09.eeg 8 5 8</t>
+  </si>
+  <si>
+    <t>Tachov/Tachov_26_3_2015_10.eeg 2 2</t>
+  </si>
+  <si>
+    <t>ZSBolevecka/ZSBolevecka_26_5_2015_01.eeg 9 9</t>
+  </si>
+  <si>
+    <t>ZSBolevecka/ZSBolevecka_26_5_2015_03.eeg 3 3</t>
+  </si>
+  <si>
+    <t>ZSBolevecka/ZSBolevecka_26_05_2015_14.eeg 6 6</t>
+  </si>
+  <si>
+    <t>ZSBolevecka/Horazdovice_26_5_2015_15.eeg 7 7</t>
+  </si>
+  <si>
+    <t>ZSBolevecka/BoleveckaZS_26_5_2015_20.eeg 3 3</t>
+  </si>
+  <si>
+    <t>ZSBolevecka/BoleveckaZS_26_5_2015_21.eeg 4 4</t>
+  </si>
+  <si>
+    <t>Tachov2/Tachov_14_5_2015_04.eeg 6 3 5 6</t>
+  </si>
+  <si>
+    <t>Tachov2/Tachov_14_5_2015_06.eeg 3 3</t>
+  </si>
+  <si>
+    <t>Tachov2/Tachov_14_5_2015_08.eeg 5 5</t>
+  </si>
+  <si>
+    <t>Tachov2/Tachov_14_05_2015_10.eeg 5 5</t>
+  </si>
+  <si>
+    <t>Tachov2/Tachov_14_5_2015_13.eeg 8 5 8</t>
+  </si>
+  <si>
+    <t>Tachov2/Tachov_14_05_2015_15.eeg 8 8</t>
+  </si>
+  <si>
+    <t>Tachov2/Tachov_14_5_2015_16.eeg 6 6</t>
+  </si>
+  <si>
+    <t>Tachov2/Tachov_14_5_2015_20.eeg 6 5 6</t>
+  </si>
+  <si>
+    <t>Tachov2/Tachov_14_5_2015_21.eeg 9 9</t>
+  </si>
+  <si>
+    <t>17ZS/17ZS_14_4_2015_13.eeg 5 5</t>
+  </si>
+  <si>
+    <t>17ZS/17ZS_14_4_2015_14.eeg 2 2</t>
+  </si>
+  <si>
+    <t>Blatnice/blatnice20141023_20.eeg 2 5 2</t>
+  </si>
+  <si>
+    <t>Blatnice/blatnice20141023_24.eeg 1 1</t>
+  </si>
+  <si>
+    <t>DolniBela/DolniBela_01.eeg 7 7</t>
+  </si>
+  <si>
+    <t>DolniBela/DolniBela_17.eeg 5 5</t>
+  </si>
+  <si>
+    <t>DolniBela/DolniBela_20.eeg 4 4</t>
+  </si>
+  <si>
+    <t>Horazdovice/Horazdovice_20140512_003.eeg 3 3</t>
+  </si>
+  <si>
+    <t>KVary/KarlovyVary_20150507_09.eeg 9 9</t>
+  </si>
+  <si>
+    <t>Masarykovo/masarykovo007_20141124.eeg 9 9</t>
+  </si>
+  <si>
+    <t>Masarykovo/masarykovo008_20141124.eeg 1 1</t>
+  </si>
+  <si>
+    <t>Stankov/Stankov_26_1_20145_27.eeg 4 4</t>
+  </si>
+  <si>
+    <t>Strasice/PD_Strasice_7_1_2015_02.eeg 5 5</t>
   </si>
 </sst>
 </file>
@@ -893,12 +898,15 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Motiv systému Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Motiv Office">
   <a:themeElements>
     <a:clrScheme name="Kancelář">
       <a:dk1>
@@ -940,7 +948,7 @@
     </a:clrScheme>
     <a:fontScheme name="Kancelář">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -975,7 +983,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1186,8 +1194,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C1:J108"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="E70" sqref="E70"/>
+    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="F108" sqref="F108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1197,15 +1205,15 @@
     <col min="3" max="3" width="33.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="33.7109375" customWidth="1"/>
     <col min="5" max="5" width="35.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="34" customWidth="1"/>
-    <col min="7" max="7" width="35.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="45.85546875" customWidth="1"/>
+    <col min="7" max="7" width="51.28515625" customWidth="1"/>
     <col min="8" max="8" width="35.28515625" customWidth="1"/>
     <col min="10" max="10" width="49.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="3:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C1" s="1" t="s">
-        <v>31</v>
+        <v>11</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>3</v>
@@ -1217,18 +1225,18 @@
         <v>0</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>38</v>
+        <v>12</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>72</v>
+        <v>22</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>41</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="D2" t="s">
         <v>1</v>
@@ -1237,995 +1245,995 @@
         <v>5</v>
       </c>
       <c r="F2" t="s">
-        <v>6</v>
+        <v>166</v>
       </c>
       <c r="G2" t="s">
-        <v>7</v>
+        <v>84</v>
       </c>
       <c r="H2" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="J2" t="s">
-        <v>42</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
-        <v>83</v>
+        <v>26</v>
       </c>
       <c r="D3" t="s">
         <v>2</v>
       </c>
       <c r="E3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F3" t="s">
-        <v>9</v>
+        <v>167</v>
       </c>
       <c r="G3" t="s">
-        <v>21</v>
+        <v>85</v>
       </c>
       <c r="H3" t="s">
-        <v>61</v>
+        <v>17</v>
       </c>
       <c r="J3" t="s">
-        <v>53</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
-        <v>136</v>
+        <v>35</v>
       </c>
       <c r="D4" t="s">
-        <v>93</v>
+        <v>28</v>
       </c>
       <c r="E4" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="F4" t="s">
-        <v>11</v>
+        <v>168</v>
       </c>
       <c r="G4" t="s">
-        <v>26</v>
+        <v>86</v>
       </c>
       <c r="H4" t="s">
-        <v>203</v>
+        <v>57</v>
       </c>
       <c r="J4" t="s">
-        <v>70</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
-        <v>147</v>
+        <v>38</v>
       </c>
       <c r="D5" t="s">
-        <v>160</v>
+        <v>42</v>
       </c>
       <c r="E5" t="s">
-        <v>27</v>
+        <v>9</v>
       </c>
       <c r="F5" t="s">
-        <v>13</v>
+        <v>169</v>
       </c>
       <c r="G5" t="s">
-        <v>28</v>
+        <v>87</v>
       </c>
       <c r="H5" t="s">
-        <v>262</v>
+        <v>78</v>
       </c>
       <c r="J5" t="s">
-        <v>71</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
-        <v>166</v>
+        <v>44</v>
       </c>
       <c r="D6" t="s">
-        <v>163</v>
+        <v>43</v>
       </c>
       <c r="E6" t="s">
-        <v>51</v>
+        <v>15</v>
       </c>
       <c r="F6" t="s">
-        <v>14</v>
+        <v>170</v>
       </c>
       <c r="G6" t="s">
-        <v>32</v>
+        <v>88</v>
       </c>
       <c r="H6" t="s">
-        <v>269</v>
+        <v>82</v>
       </c>
       <c r="J6" t="s">
-        <v>73</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
-        <v>194</v>
+        <v>54</v>
       </c>
       <c r="D7" t="s">
-        <v>179</v>
+        <v>50</v>
       </c>
       <c r="E7" t="s">
-        <v>62</v>
+        <v>18</v>
       </c>
       <c r="F7" t="s">
-        <v>15</v>
+        <v>171</v>
       </c>
       <c r="G7" t="s">
-        <v>36</v>
+        <v>89</v>
       </c>
       <c r="J7" t="s">
-        <v>74</v>
+        <v>24</v>
       </c>
     </row>
     <row r="8" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
-        <v>199</v>
+        <v>56</v>
       </c>
       <c r="D8" t="s">
-        <v>182</v>
+        <v>52</v>
       </c>
       <c r="E8" t="s">
-        <v>66</v>
+        <v>19</v>
       </c>
       <c r="F8" t="s">
-        <v>16</v>
+        <v>172</v>
       </c>
       <c r="G8" t="s">
-        <v>37</v>
+        <v>90</v>
       </c>
       <c r="J8" t="s">
-        <v>97</v>
+        <v>29</v>
       </c>
     </row>
     <row r="9" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
-        <v>222</v>
+        <v>62</v>
       </c>
       <c r="D9" t="s">
-        <v>195</v>
+        <v>55</v>
       </c>
       <c r="E9" t="s">
-        <v>76</v>
+        <v>25</v>
       </c>
       <c r="F9" t="s">
-        <v>17</v>
+        <v>173</v>
       </c>
       <c r="G9" t="s">
-        <v>39</v>
+        <v>91</v>
       </c>
       <c r="J9" t="s">
-        <v>113</v>
+        <v>31</v>
       </c>
     </row>
     <row r="10" spans="3:10" x14ac:dyDescent="0.25">
       <c r="D10" t="s">
-        <v>234</v>
+        <v>66</v>
       </c>
       <c r="E10" t="s">
-        <v>88</v>
+        <v>27</v>
       </c>
       <c r="F10" t="s">
-        <v>18</v>
+        <v>174</v>
       </c>
       <c r="G10" t="s">
-        <v>43</v>
+        <v>92</v>
       </c>
       <c r="J10" t="s">
-        <v>115</v>
+        <v>32</v>
       </c>
     </row>
     <row r="11" spans="3:10" x14ac:dyDescent="0.25">
       <c r="D11" t="s">
-        <v>235</v>
+        <v>67</v>
       </c>
       <c r="E11" t="s">
-        <v>111</v>
+        <v>30</v>
       </c>
       <c r="F11" t="s">
-        <v>19</v>
+        <v>175</v>
       </c>
       <c r="G11" t="s">
-        <v>44</v>
+        <v>93</v>
       </c>
       <c r="J11" t="s">
-        <v>124</v>
+        <v>33</v>
       </c>
     </row>
     <row r="12" spans="3:10" x14ac:dyDescent="0.25">
       <c r="D12" t="s">
-        <v>241</v>
+        <v>71</v>
       </c>
       <c r="E12" t="s">
-        <v>141</v>
+        <v>37</v>
       </c>
       <c r="F12" t="s">
-        <v>20</v>
+        <v>176</v>
       </c>
       <c r="G12" t="s">
-        <v>46</v>
+        <v>94</v>
       </c>
       <c r="J12" t="s">
-        <v>134</v>
+        <v>34</v>
       </c>
     </row>
     <row r="13" spans="3:10" x14ac:dyDescent="0.25">
       <c r="D13" t="s">
-        <v>245</v>
+        <v>73</v>
       </c>
       <c r="E13" t="s">
-        <v>155</v>
+        <v>39</v>
       </c>
       <c r="F13" t="s">
-        <v>22</v>
+        <v>177</v>
       </c>
       <c r="G13" t="s">
-        <v>47</v>
+        <v>95</v>
       </c>
       <c r="J13" t="s">
-        <v>140</v>
+        <v>36</v>
       </c>
     </row>
     <row r="14" spans="3:10" x14ac:dyDescent="0.25">
       <c r="E14" t="s">
-        <v>159</v>
+        <v>41</v>
       </c>
       <c r="F14" t="s">
-        <v>23</v>
+        <v>178</v>
       </c>
       <c r="G14" t="s">
-        <v>50</v>
+        <v>96</v>
       </c>
       <c r="J14" t="s">
-        <v>158</v>
+        <v>40</v>
       </c>
     </row>
     <row r="15" spans="3:10" x14ac:dyDescent="0.25">
       <c r="E15" t="s">
-        <v>169</v>
+        <v>45</v>
       </c>
       <c r="F15" t="s">
-        <v>24</v>
+        <v>179</v>
       </c>
       <c r="G15" t="s">
-        <v>55</v>
+        <v>97</v>
       </c>
       <c r="J15" t="s">
-        <v>171</v>
+        <v>46</v>
       </c>
     </row>
     <row r="16" spans="3:10" x14ac:dyDescent="0.25">
       <c r="E16" t="s">
-        <v>174</v>
+        <v>48</v>
       </c>
       <c r="F16" t="s">
-        <v>25</v>
+        <v>180</v>
       </c>
       <c r="G16" t="s">
-        <v>56</v>
+        <v>98</v>
       </c>
       <c r="J16" t="s">
-        <v>173</v>
+        <v>47</v>
       </c>
     </row>
     <row r="17" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E17" t="s">
-        <v>178</v>
+        <v>49</v>
       </c>
       <c r="F17" t="s">
-        <v>29</v>
+        <v>181</v>
       </c>
       <c r="G17" t="s">
-        <v>57</v>
+        <v>99</v>
       </c>
       <c r="J17" t="s">
-        <v>181</v>
+        <v>51</v>
       </c>
     </row>
     <row r="18" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E18" t="s">
-        <v>183</v>
+        <v>53</v>
       </c>
       <c r="F18" t="s">
-        <v>33</v>
+        <v>182</v>
       </c>
       <c r="G18" t="s">
+        <v>100</v>
+      </c>
+      <c r="J18" t="s">
         <v>58</v>
-      </c>
-      <c r="J18" t="s">
-        <v>204</v>
       </c>
     </row>
     <row r="19" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E19" t="s">
-        <v>209</v>
+        <v>59</v>
       </c>
       <c r="F19" t="s">
-        <v>34</v>
+        <v>183</v>
       </c>
       <c r="G19" t="s">
-        <v>59</v>
+        <v>101</v>
       </c>
       <c r="J19" t="s">
-        <v>219</v>
+        <v>61</v>
       </c>
     </row>
     <row r="20" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E20" t="s">
-        <v>210</v>
+        <v>60</v>
       </c>
       <c r="F20" t="s">
-        <v>35</v>
+        <v>184</v>
       </c>
       <c r="G20" t="s">
-        <v>63</v>
+        <v>102</v>
       </c>
       <c r="J20" t="s">
-        <v>244</v>
+        <v>72</v>
       </c>
     </row>
     <row r="21" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E21" t="s">
-        <v>228</v>
+        <v>63</v>
       </c>
       <c r="F21" t="s">
-        <v>40</v>
+        <v>185</v>
       </c>
       <c r="G21" t="s">
-        <v>67</v>
+        <v>103</v>
       </c>
       <c r="J21" t="s">
-        <v>256</v>
+        <v>77</v>
       </c>
     </row>
     <row r="22" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E22" t="s">
-        <v>230</v>
+        <v>64</v>
       </c>
       <c r="F22" t="s">
-        <v>45</v>
+        <v>186</v>
       </c>
       <c r="G22" t="s">
-        <v>77</v>
+        <v>104</v>
       </c>
       <c r="J22" t="s">
-        <v>266</v>
+        <v>79</v>
       </c>
     </row>
     <row r="23" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E23" t="s">
-        <v>233</v>
+        <v>65</v>
       </c>
       <c r="F23" t="s">
-        <v>48</v>
+        <v>187</v>
       </c>
       <c r="G23" t="s">
-        <v>78</v>
+        <v>105</v>
       </c>
       <c r="J23" t="s">
-        <v>270</v>
+        <v>83</v>
       </c>
     </row>
     <row r="24" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E24" t="s">
-        <v>238</v>
+        <v>68</v>
       </c>
       <c r="F24" t="s">
-        <v>49</v>
+        <v>188</v>
       </c>
       <c r="G24" t="s">
-        <v>96</v>
+        <v>106</v>
       </c>
     </row>
     <row r="25" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E25" t="s">
-        <v>239</v>
+        <v>69</v>
       </c>
       <c r="F25" t="s">
-        <v>52</v>
+        <v>189</v>
       </c>
       <c r="G25" t="s">
-        <v>79</v>
+        <v>107</v>
       </c>
     </row>
     <row r="26" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E26" t="s">
-        <v>240</v>
+        <v>70</v>
       </c>
       <c r="F26" t="s">
-        <v>54</v>
+        <v>190</v>
       </c>
       <c r="G26" t="s">
-        <v>81</v>
+        <v>108</v>
       </c>
     </row>
     <row r="27" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E27" t="s">
-        <v>246</v>
+        <v>74</v>
       </c>
       <c r="F27" t="s">
-        <v>69</v>
+        <v>191</v>
       </c>
       <c r="G27" t="s">
-        <v>87</v>
+        <v>109</v>
       </c>
     </row>
     <row r="28" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E28" t="s">
-        <v>247</v>
+        <v>75</v>
       </c>
       <c r="F28" t="s">
-        <v>60</v>
+        <v>192</v>
       </c>
       <c r="G28" t="s">
-        <v>89</v>
+        <v>110</v>
       </c>
     </row>
     <row r="29" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E29" t="s">
-        <v>252</v>
+        <v>76</v>
       </c>
       <c r="F29" t="s">
-        <v>64</v>
+        <v>193</v>
       </c>
       <c r="G29" t="s">
-        <v>90</v>
+        <v>111</v>
       </c>
     </row>
     <row r="30" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E30" t="s">
-        <v>267</v>
+        <v>80</v>
       </c>
       <c r="F30" t="s">
-        <v>65</v>
+        <v>194</v>
       </c>
       <c r="G30" t="s">
-        <v>91</v>
+        <v>112</v>
       </c>
     </row>
     <row r="31" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E31" t="s">
-        <v>268</v>
+        <v>81</v>
       </c>
       <c r="F31" t="s">
-        <v>68</v>
+        <v>195</v>
       </c>
       <c r="G31" t="s">
-        <v>94</v>
+        <v>113</v>
       </c>
     </row>
     <row r="32" spans="5:10" x14ac:dyDescent="0.25">
       <c r="F32" t="s">
-        <v>75</v>
+        <v>196</v>
       </c>
       <c r="G32" t="s">
-        <v>100</v>
+        <v>114</v>
       </c>
     </row>
     <row r="33" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F33" t="s">
-        <v>80</v>
+        <v>197</v>
       </c>
       <c r="G33" t="s">
-        <v>101</v>
+        <v>115</v>
       </c>
     </row>
     <row r="34" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F34" t="s">
-        <v>82</v>
+        <v>198</v>
       </c>
       <c r="G34" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
     </row>
     <row r="35" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F35" t="s">
-        <v>84</v>
+        <v>199</v>
       </c>
       <c r="G35" t="s">
-        <v>104</v>
+        <v>117</v>
       </c>
     </row>
     <row r="36" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F36" t="s">
-        <v>85</v>
+        <v>200</v>
       </c>
       <c r="G36" t="s">
-        <v>107</v>
+        <v>118</v>
       </c>
     </row>
     <row r="37" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F37" t="s">
-        <v>86</v>
+        <v>201</v>
       </c>
       <c r="G37" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
     </row>
     <row r="38" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F38" t="s">
-        <v>92</v>
+        <v>202</v>
       </c>
       <c r="G38" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
     </row>
     <row r="39" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F39" t="s">
-        <v>95</v>
+        <v>203</v>
       </c>
       <c r="G39" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
     </row>
     <row r="40" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F40" t="s">
-        <v>98</v>
+        <v>204</v>
       </c>
       <c r="G40" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
     </row>
     <row r="41" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F41" t="s">
-        <v>99</v>
+        <v>205</v>
       </c>
       <c r="G41" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
     </row>
     <row r="42" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F42" t="s">
-        <v>102</v>
+        <v>206</v>
       </c>
       <c r="G42" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
     </row>
     <row r="43" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F43" t="s">
-        <v>103</v>
+        <v>207</v>
       </c>
       <c r="G43" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
     </row>
     <row r="44" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F44" t="s">
-        <v>105</v>
+        <v>208</v>
       </c>
       <c r="G44" t="s">
-        <v>135</v>
+        <v>126</v>
       </c>
     </row>
     <row r="45" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F45" t="s">
-        <v>106</v>
+        <v>209</v>
       </c>
       <c r="G45" t="s">
-        <v>138</v>
+        <v>127</v>
       </c>
     </row>
     <row r="46" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F46" t="s">
-        <v>108</v>
+        <v>210</v>
       </c>
       <c r="G46" t="s">
-        <v>142</v>
+        <v>128</v>
       </c>
     </row>
     <row r="47" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F47" t="s">
-        <v>109</v>
+        <v>211</v>
       </c>
       <c r="G47" t="s">
-        <v>145</v>
+        <v>129</v>
       </c>
     </row>
     <row r="48" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F48" t="s">
-        <v>110</v>
+        <v>212</v>
       </c>
       <c r="G48" t="s">
-        <v>150</v>
+        <v>130</v>
       </c>
     </row>
     <row r="49" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F49" t="s">
-        <v>114</v>
+        <v>213</v>
       </c>
       <c r="G49" t="s">
-        <v>151</v>
+        <v>131</v>
       </c>
     </row>
     <row r="50" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F50" t="s">
-        <v>116</v>
+        <v>214</v>
       </c>
       <c r="G50" t="s">
-        <v>152</v>
+        <v>132</v>
       </c>
     </row>
     <row r="51" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F51" t="s">
-        <v>118</v>
+        <v>215</v>
       </c>
       <c r="G51" t="s">
-        <v>153</v>
+        <v>133</v>
       </c>
     </row>
     <row r="52" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F52" t="s">
-        <v>120</v>
+        <v>216</v>
       </c>
       <c r="G52" t="s">
-        <v>161</v>
+        <v>134</v>
       </c>
     </row>
     <row r="53" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F53" t="s">
-        <v>121</v>
+        <v>217</v>
       </c>
       <c r="G53" t="s">
-        <v>162</v>
+        <v>135</v>
       </c>
     </row>
     <row r="54" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F54" t="s">
-        <v>122</v>
+        <v>218</v>
       </c>
       <c r="G54" t="s">
-        <v>165</v>
+        <v>136</v>
       </c>
     </row>
     <row r="55" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F55" t="s">
-        <v>123</v>
+        <v>219</v>
       </c>
       <c r="G55" t="s">
-        <v>167</v>
+        <v>137</v>
       </c>
     </row>
     <row r="56" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F56" t="s">
-        <v>126</v>
+        <v>220</v>
       </c>
       <c r="G56" t="s">
-        <v>168</v>
+        <v>138</v>
       </c>
     </row>
     <row r="57" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F57" t="s">
-        <v>127</v>
+        <v>221</v>
       </c>
       <c r="G57" t="s">
-        <v>175</v>
+        <v>139</v>
       </c>
     </row>
     <row r="58" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F58" t="s">
-        <v>130</v>
+        <v>222</v>
       </c>
       <c r="G58" t="s">
-        <v>177</v>
+        <v>140</v>
       </c>
     </row>
     <row r="59" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F59" t="s">
-        <v>133</v>
+        <v>223</v>
       </c>
       <c r="G59" t="s">
-        <v>186</v>
+        <v>141</v>
       </c>
     </row>
     <row r="60" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F60" t="s">
-        <v>137</v>
+        <v>224</v>
       </c>
       <c r="G60" t="s">
-        <v>188</v>
+        <v>142</v>
       </c>
     </row>
     <row r="61" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F61" t="s">
-        <v>139</v>
+        <v>225</v>
       </c>
       <c r="G61" t="s">
-        <v>189</v>
+        <v>143</v>
       </c>
     </row>
     <row r="62" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F62" t="s">
-        <v>143</v>
+        <v>226</v>
       </c>
       <c r="G62" t="s">
-        <v>191</v>
+        <v>144</v>
       </c>
     </row>
     <row r="63" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F63" t="s">
-        <v>144</v>
+        <v>227</v>
       </c>
       <c r="G63" t="s">
-        <v>196</v>
+        <v>145</v>
       </c>
     </row>
     <row r="64" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F64" t="s">
+        <v>228</v>
+      </c>
+      <c r="G64" t="s">
         <v>146</v>
-      </c>
-      <c r="G64" t="s">
-        <v>200</v>
       </c>
     </row>
     <row r="65" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F65" t="s">
-        <v>148</v>
+        <v>229</v>
       </c>
       <c r="G65" t="s">
-        <v>201</v>
+        <v>147</v>
       </c>
     </row>
     <row r="66" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F66" t="s">
-        <v>149</v>
+        <v>230</v>
       </c>
       <c r="G66" t="s">
-        <v>205</v>
+        <v>148</v>
       </c>
     </row>
     <row r="67" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F67" t="s">
-        <v>154</v>
+        <v>231</v>
       </c>
       <c r="G67" t="s">
-        <v>206</v>
+        <v>149</v>
       </c>
     </row>
     <row r="68" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F68" t="s">
-        <v>156</v>
+        <v>232</v>
       </c>
       <c r="G68" t="s">
-        <v>211</v>
+        <v>150</v>
       </c>
     </row>
     <row r="69" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F69" t="s">
-        <v>157</v>
+        <v>233</v>
       </c>
       <c r="G69" t="s">
-        <v>213</v>
+        <v>151</v>
       </c>
     </row>
     <row r="70" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F70" t="s">
-        <v>164</v>
+        <v>234</v>
       </c>
       <c r="G70" t="s">
-        <v>214</v>
+        <v>152</v>
       </c>
     </row>
     <row r="71" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F71" t="s">
-        <v>170</v>
+        <v>235</v>
       </c>
       <c r="G71" t="s">
-        <v>215</v>
+        <v>153</v>
       </c>
     </row>
     <row r="72" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F72" t="s">
-        <v>172</v>
+        <v>236</v>
       </c>
       <c r="G72" t="s">
-        <v>221</v>
+        <v>154</v>
       </c>
     </row>
     <row r="73" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F73" t="s">
-        <v>176</v>
+        <v>237</v>
       </c>
       <c r="G73" t="s">
-        <v>223</v>
+        <v>155</v>
       </c>
     </row>
     <row r="74" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F74" t="s">
-        <v>180</v>
+        <v>238</v>
       </c>
       <c r="G74" t="s">
-        <v>224</v>
+        <v>156</v>
       </c>
     </row>
     <row r="75" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F75" t="s">
-        <v>184</v>
+        <v>239</v>
       </c>
       <c r="G75" t="s">
-        <v>232</v>
+        <v>157</v>
       </c>
     </row>
     <row r="76" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F76" t="s">
-        <v>185</v>
+        <v>240</v>
       </c>
       <c r="G76" t="s">
-        <v>236</v>
+        <v>158</v>
       </c>
     </row>
     <row r="77" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F77" t="s">
-        <v>187</v>
+        <v>241</v>
       </c>
       <c r="G77" t="s">
-        <v>237</v>
+        <v>159</v>
       </c>
     </row>
     <row r="78" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F78" t="s">
-        <v>190</v>
+        <v>242</v>
       </c>
       <c r="G78" t="s">
-        <v>250</v>
+        <v>160</v>
       </c>
     </row>
     <row r="79" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F79" t="s">
-        <v>192</v>
+        <v>243</v>
       </c>
       <c r="G79" t="s">
-        <v>251</v>
+        <v>161</v>
       </c>
     </row>
     <row r="80" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F80" t="s">
-        <v>193</v>
+        <v>244</v>
       </c>
       <c r="G80" t="s">
-        <v>254</v>
+        <v>162</v>
       </c>
     </row>
     <row r="81" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F81" t="s">
-        <v>197</v>
+        <v>245</v>
       </c>
       <c r="G81" t="s">
-        <v>257</v>
+        <v>163</v>
       </c>
     </row>
     <row r="82" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F82" t="s">
-        <v>198</v>
+        <v>246</v>
       </c>
       <c r="G82" t="s">
-        <v>259</v>
+        <v>164</v>
       </c>
     </row>
     <row r="83" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F83" t="s">
-        <v>202</v>
+        <v>247</v>
       </c>
       <c r="G83" t="s">
-        <v>261</v>
+        <v>165</v>
       </c>
     </row>
     <row r="84" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F84" t="s">
-        <v>207</v>
+        <v>248</v>
       </c>
     </row>
     <row r="85" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F85" t="s">
-        <v>208</v>
+        <v>249</v>
       </c>
     </row>
     <row r="86" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F86" t="s">
-        <v>212</v>
+        <v>250</v>
       </c>
     </row>
     <row r="87" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F87" t="s">
-        <v>216</v>
+        <v>251</v>
       </c>
     </row>
     <row r="88" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F88" t="s">
-        <v>217</v>
+        <v>252</v>
       </c>
     </row>
     <row r="89" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F89" t="s">
-        <v>218</v>
+        <v>253</v>
       </c>
     </row>
     <row r="90" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F90" t="s">
-        <v>220</v>
+        <v>254</v>
       </c>
     </row>
     <row r="91" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F91" t="s">
-        <v>225</v>
+        <v>255</v>
       </c>
     </row>
     <row r="92" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F92" t="s">
-        <v>226</v>
+        <v>256</v>
       </c>
     </row>
     <row r="93" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F93" t="s">
-        <v>227</v>
+        <v>257</v>
       </c>
     </row>
     <row r="94" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F94" t="s">
-        <v>229</v>
+        <v>258</v>
       </c>
     </row>
     <row r="95" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F95" t="s">
-        <v>231</v>
+        <v>259</v>
       </c>
     </row>
     <row r="96" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F96" t="s">
-        <v>242</v>
+        <v>260</v>
       </c>
     </row>
     <row r="97" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F97" t="s">
-        <v>243</v>
+        <v>261</v>
       </c>
     </row>
     <row r="98" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F98" t="s">
-        <v>248</v>
+        <v>262</v>
       </c>
     </row>
     <row r="99" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F99" t="s">
-        <v>249</v>
+        <v>263</v>
       </c>
     </row>
     <row r="100" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F100" t="s">
-        <v>253</v>
+        <v>264</v>
       </c>
     </row>
     <row r="101" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F101" t="s">
-        <v>255</v>
+        <v>265</v>
       </c>
     </row>
     <row r="102" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F102" t="s">
-        <v>258</v>
+        <v>266</v>
       </c>
     </row>
     <row r="103" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F103" t="s">
-        <v>260</v>
+        <v>267</v>
       </c>
     </row>
     <row r="104" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F104" t="s">
-        <v>263</v>
+        <v>268</v>
       </c>
     </row>
     <row r="105" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F105" t="s">
-        <v>264</v>
+        <v>269</v>
       </c>
     </row>
     <row r="106" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F106" t="s">
-        <v>265</v>
+        <v>270</v>
       </c>
     </row>
     <row r="107" spans="6:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
rozdeleni_dat and info updated. unused import removed
</commit_message>
<xml_diff>
--- a/rozdeleni_dat.xlsx
+++ b/rozdeleni_dat.xlsx
@@ -38,21 +38,9 @@
     <t>méně rozkmitané</t>
   </si>
   <si>
-    <t>17ZS_14_4_2015_03.eeg 6 2 6</t>
-  </si>
-  <si>
-    <t>17ZS_14_4_2015_6.eeg 8 8</t>
-  </si>
-  <si>
-    <t>17ZS_14_4_2015_8.eeg 4 4</t>
-  </si>
-  <si>
     <t>17ZS_14_4_2015_10.eeg 2 2</t>
   </si>
   <si>
-    <t>blastnice_20141023_21.eeg 1 1</t>
-  </si>
-  <si>
     <t>blatnice20141023_8.eeg 1 1</t>
   </si>
   <si>
@@ -68,21 +56,12 @@
     <t>Blatnice - divný 1. kanál</t>
   </si>
   <si>
-    <t>DolniBela_03.eeg 2 2</t>
-  </si>
-  <si>
     <t>DolniBela_04.eeg - kopec dolů</t>
   </si>
   <si>
     <t>DolniBela_13.eeg 3 3</t>
   </si>
   <si>
-    <t>DolniBela_14.eeg 5 1</t>
-  </si>
-  <si>
-    <t>DolniBela_18.eeg 4 4</t>
-  </si>
-  <si>
     <t>DolniBela_06.eeg - kopec dolů</t>
   </si>
   <si>
@@ -98,24 +77,15 @@
     <t>DolniBela_16.eeg - kopec dolů</t>
   </si>
   <si>
-    <t>Horazdovice_20141205_001.eeg 4 9 3 4</t>
-  </si>
-  <si>
     <t>Horazdovice_20141204_017.eeg 3 7 3</t>
   </si>
   <si>
-    <t>Horazdovice20141204_023.eeg 2 2</t>
-  </si>
-  <si>
     <t>Horazdovice20141204_030.eeg 2 2</t>
   </si>
   <si>
     <t>Horazdovice_20141204_018.eeg - rozkmitaná</t>
   </si>
   <si>
-    <t>KarlovyVary_20150507_15.eeg 4 4</t>
-  </si>
-  <si>
     <t>KarlovyVary_20150507_10.eeg - rozkmitaná</t>
   </si>
   <si>
@@ -134,21 +104,12 @@
     <t>SPSD_3_2_2015_03.eeg - neuhádnuto</t>
   </si>
   <si>
-    <t>SPSD_3_2_2015_04.eeg 1 4 1</t>
-  </si>
-  <si>
     <t>SPSD_3_2_2015_10.eeg 3 7 3</t>
   </si>
   <si>
-    <t>Stankov_26_01_2015_08.eeg 5 5</t>
-  </si>
-  <si>
     <t>Stankov_26_1_2015_10.eeg - kopec dolů</t>
   </si>
   <si>
-    <t>Stankov_26_01_2015_11.eeg 3 4 3</t>
-  </si>
-  <si>
     <t>Stankov_26_1_2015_12.eeg 5 9 6 3</t>
   </si>
   <si>
@@ -158,21 +119,12 @@
     <t>Stankov_26_1_2015_18.eeg 8 5 1 8</t>
   </si>
   <si>
-    <t>Stankov_26_01_2015_21.eeg 6 6</t>
-  </si>
-  <si>
     <t>Stankov_26_01_2015_22.eeg - rozkmitaná</t>
   </si>
   <si>
     <t>Stankov_26_1_2015_23.eeg -  rozkmitaná</t>
   </si>
   <si>
-    <t>Stankov_26_1_2015_24.eeg 5 5</t>
-  </si>
-  <si>
-    <t>Stankov_26_1_2015_29.eeg 9 1</t>
-  </si>
-  <si>
     <t>pd_strasice_7_1_2015_01.eeg 3 3</t>
   </si>
   <si>
@@ -182,9 +134,6 @@
     <t>PD_Strasice_7_1_2015_03.eeg 5 5</t>
   </si>
   <si>
-    <t>PD_Strasice_7_1_2015_04.eeg 5 5</t>
-  </si>
-  <si>
     <t>PD_Strasice_7_2015_15.eeg 8 8</t>
   </si>
   <si>
@@ -200,42 +149,18 @@
     <t>Strasice_4_2_2015_10.eeg  - stejný popis jako u 09</t>
   </si>
   <si>
-    <t>Strasice_4_2_2015_15.eeg 3 3</t>
-  </si>
-  <si>
-    <t>Strasice_4_2_2015_16.eeg 2 3 2</t>
-  </si>
-  <si>
     <t>Tachov_26_3_2015_02.eeg - kopec dolů</t>
   </si>
   <si>
     <t>Tachov_26_3_2015_05.eeg 2 1 9 6</t>
   </si>
   <si>
-    <t>Tachov_26_3_2015_11.eeg 2 8 1</t>
-  </si>
-  <si>
-    <t>ZSBolevecka_26_5_2015_02.eeg 5 5</t>
-  </si>
-  <si>
-    <t>ZSBolevecka_26_5_2015_05.eeg 8 8</t>
-  </si>
-  <si>
     <t>ZSBolevecka_26_5_2015_06.eeg 5 7</t>
   </si>
   <si>
     <t>BoleveckaZS_26_5_2015_07.eeg 3 9</t>
   </si>
   <si>
-    <t>ZSBolevec_26_5_2015_10.eeg 6 4 9 7</t>
-  </si>
-  <si>
-    <t>ZSBolevecka_26_5_2015_11.eeg 7 7</t>
-  </si>
-  <si>
-    <t>ZSBolevecka_26_5_2015_12.eeg 3 3</t>
-  </si>
-  <si>
     <t>BoleveckaZS_26_5_2015_13.eeg 7 7</t>
   </si>
   <si>
@@ -245,15 +170,6 @@
     <t>ZSBolevecka_26_5_2015_16.eeg 6 9 7 3</t>
   </si>
   <si>
-    <t>ZSBolevecka_26_5_2015_17.eeg 6 4 9 6</t>
-  </si>
-  <si>
-    <t>BoleveckaZS_26_5_2015_19.eeg 7 4</t>
-  </si>
-  <si>
-    <t>Tachov_14_05_2015_03.eeg 2 5 3</t>
-  </si>
-  <si>
     <t>Tachov_14_5_2015_06.eeg - rozkmitaná</t>
   </si>
   <si>
@@ -263,12 +179,6 @@
     <t>Tachov_14_5_2015_16.eeg mírně rozkmitaná</t>
   </si>
   <si>
-    <t>Tachov_14_5_2015_17.eeg 7 3 7</t>
-  </si>
-  <si>
-    <t>Tachov_14_5_2015_18.eeg 7 5 7</t>
-  </si>
-  <si>
     <t>Tachov_14_5_2015_19.eeg 7 5 7</t>
   </si>
   <si>
@@ -840,6 +750,96 @@
   </si>
   <si>
     <t>Strasice/PD_Strasice_7_1_2015_02.eeg 5 5</t>
+  </si>
+  <si>
+    <t>17ZS/17ZS_14_4_2015_03.eeg 6 2 6</t>
+  </si>
+  <si>
+    <t>17ZS/17ZS_14_4_2015_6.eeg 8 8</t>
+  </si>
+  <si>
+    <t>17ZS/17ZS_14_4_2015_8.eeg 4 4</t>
+  </si>
+  <si>
+    <t>Blatnice/blastnice_20141023_21.eeg 1 1</t>
+  </si>
+  <si>
+    <t>DolniBela/DolniBela_03.eeg 2 2</t>
+  </si>
+  <si>
+    <t>DolniBela/DolniBela_14.eeg 5 1</t>
+  </si>
+  <si>
+    <t>DolniBela/DolniBela_18.eeg 4 4</t>
+  </si>
+  <si>
+    <t>Horazdovice/Horazdovice_20141205_001.eeg 4 9 3 4</t>
+  </si>
+  <si>
+    <t>Horazdovice/Horazdovice20141204_023.eeg 2 2</t>
+  </si>
+  <si>
+    <t>KVary/KarlovyVary_20150507_15.eeg 4 4</t>
+  </si>
+  <si>
+    <t>SPSD/SPSD_3_2_2015_04.eeg 1 4 1</t>
+  </si>
+  <si>
+    <t>Stankov/Stankov_26_01_2015_08.eeg 5 5</t>
+  </si>
+  <si>
+    <t>Stankov/Stankov_26_01_2015_11.eeg 3 4 3</t>
+  </si>
+  <si>
+    <t>Stankov/Stankov_26_01_2015_21.eeg 6 6</t>
+  </si>
+  <si>
+    <t>Stankov/Stankov_26_1_2015_24.eeg 5 5</t>
+  </si>
+  <si>
+    <t>Stankov/Stankov_26_1_2015_29.eeg 9 1</t>
+  </si>
+  <si>
+    <t>Strasice/PD_Strasice_7_1_2015_04.eeg 5 5</t>
+  </si>
+  <si>
+    <t>Strasice2/Strasice_4_2_2015_15.eeg 3 3</t>
+  </si>
+  <si>
+    <t>Strasice2/Strasice_4_2_2015_16.eeg 2 3 2</t>
+  </si>
+  <si>
+    <t>Tachov/Tachov_26_3_2015_11.eeg 2 8 1</t>
+  </si>
+  <si>
+    <t>ZSBolevecka/ZSBolevecka_26_5_2015_02.eeg 5 5</t>
+  </si>
+  <si>
+    <t>ZSBolevecka/ZSBolevecka_26_5_2015_05.eeg 8 8</t>
+  </si>
+  <si>
+    <t>ZSBolevecka/ZSBolevec_26_5_2015_10.eeg 6 4 9 7</t>
+  </si>
+  <si>
+    <t>ZSBolevecka/ZSBolevecka_26_5_2015_11.eeg 7 7</t>
+  </si>
+  <si>
+    <t>ZSBolevecka/ZSBolevecka_26_5_2015_12.eeg 3 3</t>
+  </si>
+  <si>
+    <t>ZSBolevecka/ZSBolevecka_26_5_2015_17.eeg 6 4 9 6</t>
+  </si>
+  <si>
+    <t>ZSBolevecka/BoleveckaZS_26_5_2015_19.eeg 7 4</t>
+  </si>
+  <si>
+    <t>Tachov2/Tachov_14_05_2015_03.eeg 2 5 3</t>
+  </si>
+  <si>
+    <t>Tachov2/Tachov_14_5_2015_17.eeg 7 3 7</t>
+  </si>
+  <si>
+    <t>Tachov2/Tachov_14_5_2015_18.eeg 7 5 7</t>
   </si>
 </sst>
 </file>
@@ -1195,7 +1195,7 @@
   <dimension ref="C1:J108"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="F108" sqref="F108"/>
+      <selection activeCell="E31" sqref="E2:E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1204,7 +1204,7 @@
     <col min="2" max="2" width="4.7109375" customWidth="1"/>
     <col min="3" max="3" width="33.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="33.7109375" customWidth="1"/>
-    <col min="5" max="5" width="35.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="49.5703125" customWidth="1"/>
     <col min="6" max="6" width="45.85546875" customWidth="1"/>
     <col min="7" max="7" width="51.28515625" customWidth="1"/>
     <col min="8" max="8" width="35.28515625" customWidth="1"/>
@@ -1213,7 +1213,7 @@
   <sheetData>
     <row r="1" spans="3:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C1" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>3</v>
@@ -1225,1025 +1225,1025 @@
         <v>0</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="D2" t="s">
         <v>1</v>
       </c>
       <c r="E2" t="s">
+        <v>243</v>
+      </c>
+      <c r="F2" t="s">
+        <v>136</v>
+      </c>
+      <c r="G2" t="s">
+        <v>54</v>
+      </c>
+      <c r="H2" t="s">
         <v>5</v>
       </c>
-      <c r="F2" t="s">
-        <v>166</v>
-      </c>
-      <c r="G2" t="s">
-        <v>84</v>
-      </c>
-      <c r="H2" t="s">
-        <v>8</v>
-      </c>
       <c r="J2" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="D3" t="s">
         <v>2</v>
       </c>
       <c r="E3" t="s">
-        <v>6</v>
+        <v>244</v>
       </c>
       <c r="F3" t="s">
-        <v>167</v>
+        <v>137</v>
       </c>
       <c r="G3" t="s">
-        <v>85</v>
+        <v>55</v>
       </c>
       <c r="H3" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="J3" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="D4" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="E4" t="s">
-        <v>7</v>
+        <v>245</v>
       </c>
       <c r="F4" t="s">
-        <v>168</v>
+        <v>138</v>
       </c>
       <c r="G4" t="s">
-        <v>86</v>
+        <v>56</v>
       </c>
       <c r="H4" t="s">
-        <v>57</v>
+        <v>40</v>
       </c>
       <c r="J4" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="D5" t="s">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="E5" t="s">
-        <v>9</v>
+        <v>246</v>
       </c>
       <c r="F5" t="s">
-        <v>169</v>
+        <v>139</v>
       </c>
       <c r="G5" t="s">
-        <v>87</v>
+        <v>57</v>
       </c>
       <c r="H5" t="s">
-        <v>78</v>
+        <v>50</v>
       </c>
       <c r="J5" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
-        <v>44</v>
+        <v>31</v>
       </c>
       <c r="D6" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="E6" t="s">
-        <v>15</v>
+        <v>247</v>
       </c>
       <c r="F6" t="s">
-        <v>170</v>
+        <v>140</v>
       </c>
       <c r="G6" t="s">
-        <v>88</v>
+        <v>58</v>
       </c>
       <c r="H6" t="s">
-        <v>82</v>
+        <v>52</v>
       </c>
       <c r="J6" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
-        <v>54</v>
+        <v>37</v>
       </c>
       <c r="D7" t="s">
-        <v>50</v>
+        <v>34</v>
       </c>
       <c r="E7" t="s">
-        <v>18</v>
+        <v>248</v>
       </c>
       <c r="F7" t="s">
-        <v>171</v>
+        <v>141</v>
       </c>
       <c r="G7" t="s">
-        <v>89</v>
+        <v>59</v>
       </c>
       <c r="J7" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
-        <v>56</v>
+        <v>39</v>
       </c>
       <c r="D8" t="s">
-        <v>52</v>
+        <v>36</v>
       </c>
       <c r="E8" t="s">
-        <v>19</v>
+        <v>249</v>
       </c>
       <c r="F8" t="s">
-        <v>172</v>
+        <v>142</v>
       </c>
       <c r="G8" t="s">
-        <v>90</v>
+        <v>60</v>
       </c>
       <c r="J8" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
-        <v>62</v>
+        <v>43</v>
       </c>
       <c r="D9" t="s">
-        <v>55</v>
+        <v>38</v>
       </c>
       <c r="E9" t="s">
-        <v>25</v>
+        <v>250</v>
       </c>
       <c r="F9" t="s">
-        <v>173</v>
+        <v>143</v>
       </c>
       <c r="G9" t="s">
-        <v>91</v>
+        <v>61</v>
       </c>
       <c r="J9" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
     </row>
     <row r="10" spans="3:10" x14ac:dyDescent="0.25">
       <c r="D10" t="s">
-        <v>66</v>
+        <v>44</v>
       </c>
       <c r="E10" t="s">
-        <v>27</v>
+        <v>251</v>
       </c>
       <c r="F10" t="s">
-        <v>174</v>
+        <v>144</v>
       </c>
       <c r="G10" t="s">
-        <v>92</v>
+        <v>62</v>
       </c>
       <c r="J10" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
     </row>
     <row r="11" spans="3:10" x14ac:dyDescent="0.25">
       <c r="D11" t="s">
-        <v>67</v>
+        <v>45</v>
       </c>
       <c r="E11" t="s">
-        <v>30</v>
+        <v>252</v>
       </c>
       <c r="F11" t="s">
-        <v>175</v>
+        <v>145</v>
       </c>
       <c r="G11" t="s">
-        <v>93</v>
+        <v>63</v>
       </c>
       <c r="J11" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
     </row>
     <row r="12" spans="3:10" x14ac:dyDescent="0.25">
       <c r="D12" t="s">
-        <v>71</v>
+        <v>46</v>
       </c>
       <c r="E12" t="s">
-        <v>37</v>
+        <v>253</v>
       </c>
       <c r="F12" t="s">
-        <v>176</v>
+        <v>146</v>
       </c>
       <c r="G12" t="s">
-        <v>94</v>
+        <v>64</v>
       </c>
       <c r="J12" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
     </row>
     <row r="13" spans="3:10" x14ac:dyDescent="0.25">
       <c r="D13" t="s">
-        <v>73</v>
+        <v>48</v>
       </c>
       <c r="E13" t="s">
-        <v>39</v>
+        <v>254</v>
       </c>
       <c r="F13" t="s">
-        <v>177</v>
+        <v>147</v>
       </c>
       <c r="G13" t="s">
-        <v>95</v>
+        <v>65</v>
       </c>
       <c r="J13" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
     </row>
     <row r="14" spans="3:10" x14ac:dyDescent="0.25">
       <c r="E14" t="s">
-        <v>41</v>
+        <v>255</v>
       </c>
       <c r="F14" t="s">
-        <v>178</v>
+        <v>148</v>
       </c>
       <c r="G14" t="s">
-        <v>96</v>
+        <v>66</v>
       </c>
       <c r="J14" t="s">
-        <v>40</v>
+        <v>28</v>
       </c>
     </row>
     <row r="15" spans="3:10" x14ac:dyDescent="0.25">
       <c r="E15" t="s">
-        <v>45</v>
+        <v>256</v>
       </c>
       <c r="F15" t="s">
-        <v>179</v>
+        <v>149</v>
       </c>
       <c r="G15" t="s">
-        <v>97</v>
+        <v>67</v>
       </c>
       <c r="J15" t="s">
-        <v>46</v>
+        <v>32</v>
       </c>
     </row>
     <row r="16" spans="3:10" x14ac:dyDescent="0.25">
       <c r="E16" t="s">
-        <v>48</v>
+        <v>257</v>
       </c>
       <c r="F16" t="s">
-        <v>180</v>
+        <v>150</v>
       </c>
       <c r="G16" t="s">
-        <v>98</v>
+        <v>68</v>
       </c>
       <c r="J16" t="s">
-        <v>47</v>
+        <v>33</v>
       </c>
     </row>
     <row r="17" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E17" t="s">
-        <v>49</v>
+        <v>258</v>
       </c>
       <c r="F17" t="s">
-        <v>181</v>
+        <v>151</v>
       </c>
       <c r="G17" t="s">
-        <v>99</v>
+        <v>69</v>
       </c>
       <c r="J17" t="s">
-        <v>51</v>
+        <v>35</v>
       </c>
     </row>
     <row r="18" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E18" t="s">
-        <v>53</v>
+        <v>259</v>
       </c>
       <c r="F18" t="s">
-        <v>182</v>
+        <v>152</v>
       </c>
       <c r="G18" t="s">
-        <v>100</v>
+        <v>70</v>
       </c>
       <c r="J18" t="s">
-        <v>58</v>
+        <v>41</v>
       </c>
     </row>
     <row r="19" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E19" t="s">
-        <v>59</v>
+        <v>260</v>
       </c>
       <c r="F19" t="s">
-        <v>183</v>
+        <v>153</v>
       </c>
       <c r="G19" t="s">
-        <v>101</v>
+        <v>71</v>
       </c>
       <c r="J19" t="s">
-        <v>61</v>
+        <v>42</v>
       </c>
     </row>
     <row r="20" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E20" t="s">
-        <v>60</v>
+        <v>261</v>
       </c>
       <c r="F20" t="s">
-        <v>184</v>
+        <v>154</v>
       </c>
       <c r="G20" t="s">
-        <v>102</v>
+        <v>72</v>
       </c>
       <c r="J20" t="s">
-        <v>72</v>
+        <v>47</v>
       </c>
     </row>
     <row r="21" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E21" t="s">
-        <v>63</v>
+        <v>262</v>
       </c>
       <c r="F21" t="s">
-        <v>185</v>
+        <v>155</v>
       </c>
       <c r="G21" t="s">
-        <v>103</v>
+        <v>73</v>
       </c>
       <c r="J21" t="s">
-        <v>77</v>
+        <v>49</v>
       </c>
     </row>
     <row r="22" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E22" t="s">
-        <v>64</v>
+        <v>263</v>
       </c>
       <c r="F22" t="s">
-        <v>186</v>
+        <v>156</v>
       </c>
       <c r="G22" t="s">
-        <v>104</v>
+        <v>74</v>
       </c>
       <c r="J22" t="s">
-        <v>79</v>
+        <v>51</v>
       </c>
     </row>
     <row r="23" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E23" t="s">
-        <v>65</v>
+        <v>264</v>
       </c>
       <c r="F23" t="s">
-        <v>187</v>
+        <v>157</v>
       </c>
       <c r="G23" t="s">
-        <v>105</v>
+        <v>75</v>
       </c>
       <c r="J23" t="s">
-        <v>83</v>
+        <v>53</v>
       </c>
     </row>
     <row r="24" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E24" t="s">
-        <v>68</v>
+        <v>265</v>
       </c>
       <c r="F24" t="s">
-        <v>188</v>
+        <v>158</v>
       </c>
       <c r="G24" t="s">
-        <v>106</v>
+        <v>76</v>
       </c>
     </row>
     <row r="25" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E25" t="s">
-        <v>69</v>
+        <v>266</v>
       </c>
       <c r="F25" t="s">
-        <v>189</v>
+        <v>159</v>
       </c>
       <c r="G25" t="s">
-        <v>107</v>
+        <v>77</v>
       </c>
     </row>
     <row r="26" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E26" t="s">
-        <v>70</v>
+        <v>267</v>
       </c>
       <c r="F26" t="s">
-        <v>190</v>
+        <v>160</v>
       </c>
       <c r="G26" t="s">
-        <v>108</v>
+        <v>78</v>
       </c>
     </row>
     <row r="27" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E27" t="s">
-        <v>74</v>
+        <v>268</v>
       </c>
       <c r="F27" t="s">
-        <v>191</v>
+        <v>161</v>
       </c>
       <c r="G27" t="s">
-        <v>109</v>
+        <v>79</v>
       </c>
     </row>
     <row r="28" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E28" t="s">
-        <v>75</v>
+        <v>269</v>
       </c>
       <c r="F28" t="s">
-        <v>192</v>
+        <v>162</v>
       </c>
       <c r="G28" t="s">
-        <v>110</v>
+        <v>80</v>
       </c>
     </row>
     <row r="29" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E29" t="s">
-        <v>76</v>
+        <v>270</v>
       </c>
       <c r="F29" t="s">
-        <v>193</v>
+        <v>163</v>
       </c>
       <c r="G29" t="s">
-        <v>111</v>
+        <v>81</v>
       </c>
     </row>
     <row r="30" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E30" t="s">
-        <v>80</v>
+        <v>271</v>
       </c>
       <c r="F30" t="s">
-        <v>194</v>
+        <v>164</v>
       </c>
       <c r="G30" t="s">
-        <v>112</v>
+        <v>82</v>
       </c>
     </row>
     <row r="31" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E31" t="s">
-        <v>81</v>
+        <v>272</v>
       </c>
       <c r="F31" t="s">
-        <v>195</v>
+        <v>165</v>
       </c>
       <c r="G31" t="s">
-        <v>113</v>
+        <v>83</v>
       </c>
     </row>
     <row r="32" spans="5:10" x14ac:dyDescent="0.25">
       <c r="F32" t="s">
-        <v>196</v>
+        <v>166</v>
       </c>
       <c r="G32" t="s">
-        <v>114</v>
+        <v>84</v>
       </c>
     </row>
     <row r="33" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F33" t="s">
-        <v>197</v>
+        <v>167</v>
       </c>
       <c r="G33" t="s">
-        <v>115</v>
+        <v>85</v>
       </c>
     </row>
     <row r="34" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F34" t="s">
-        <v>198</v>
+        <v>168</v>
       </c>
       <c r="G34" t="s">
-        <v>116</v>
+        <v>86</v>
       </c>
     </row>
     <row r="35" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F35" t="s">
-        <v>199</v>
+        <v>169</v>
       </c>
       <c r="G35" t="s">
-        <v>117</v>
+        <v>87</v>
       </c>
     </row>
     <row r="36" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F36" t="s">
-        <v>200</v>
+        <v>170</v>
       </c>
       <c r="G36" t="s">
-        <v>118</v>
+        <v>88</v>
       </c>
     </row>
     <row r="37" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F37" t="s">
-        <v>201</v>
+        <v>171</v>
       </c>
       <c r="G37" t="s">
-        <v>119</v>
+        <v>89</v>
       </c>
     </row>
     <row r="38" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F38" t="s">
-        <v>202</v>
+        <v>172</v>
       </c>
       <c r="G38" t="s">
-        <v>120</v>
+        <v>90</v>
       </c>
     </row>
     <row r="39" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F39" t="s">
-        <v>203</v>
+        <v>173</v>
       </c>
       <c r="G39" t="s">
-        <v>121</v>
+        <v>91</v>
       </c>
     </row>
     <row r="40" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F40" t="s">
-        <v>204</v>
+        <v>174</v>
       </c>
       <c r="G40" t="s">
-        <v>122</v>
+        <v>92</v>
       </c>
     </row>
     <row r="41" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F41" t="s">
-        <v>205</v>
+        <v>175</v>
       </c>
       <c r="G41" t="s">
-        <v>123</v>
+        <v>93</v>
       </c>
     </row>
     <row r="42" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F42" t="s">
-        <v>206</v>
+        <v>176</v>
       </c>
       <c r="G42" t="s">
-        <v>124</v>
+        <v>94</v>
       </c>
     </row>
     <row r="43" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F43" t="s">
-        <v>207</v>
+        <v>177</v>
       </c>
       <c r="G43" t="s">
-        <v>125</v>
+        <v>95</v>
       </c>
     </row>
     <row r="44" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F44" t="s">
-        <v>208</v>
+        <v>178</v>
       </c>
       <c r="G44" t="s">
-        <v>126</v>
+        <v>96</v>
       </c>
     </row>
     <row r="45" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F45" t="s">
-        <v>209</v>
+        <v>179</v>
       </c>
       <c r="G45" t="s">
-        <v>127</v>
+        <v>97</v>
       </c>
     </row>
     <row r="46" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F46" t="s">
-        <v>210</v>
+        <v>180</v>
       </c>
       <c r="G46" t="s">
-        <v>128</v>
+        <v>98</v>
       </c>
     </row>
     <row r="47" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F47" t="s">
-        <v>211</v>
+        <v>181</v>
       </c>
       <c r="G47" t="s">
-        <v>129</v>
+        <v>99</v>
       </c>
     </row>
     <row r="48" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F48" t="s">
-        <v>212</v>
+        <v>182</v>
       </c>
       <c r="G48" t="s">
-        <v>130</v>
+        <v>100</v>
       </c>
     </row>
     <row r="49" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F49" t="s">
-        <v>213</v>
+        <v>183</v>
       </c>
       <c r="G49" t="s">
-        <v>131</v>
+        <v>101</v>
       </c>
     </row>
     <row r="50" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F50" t="s">
-        <v>214</v>
+        <v>184</v>
       </c>
       <c r="G50" t="s">
-        <v>132</v>
+        <v>102</v>
       </c>
     </row>
     <row r="51" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F51" t="s">
-        <v>215</v>
+        <v>185</v>
       </c>
       <c r="G51" t="s">
-        <v>133</v>
+        <v>103</v>
       </c>
     </row>
     <row r="52" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F52" t="s">
-        <v>216</v>
+        <v>186</v>
       </c>
       <c r="G52" t="s">
-        <v>134</v>
+        <v>104</v>
       </c>
     </row>
     <row r="53" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F53" t="s">
-        <v>217</v>
+        <v>187</v>
       </c>
       <c r="G53" t="s">
-        <v>135</v>
+        <v>105</v>
       </c>
     </row>
     <row r="54" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F54" t="s">
-        <v>218</v>
+        <v>188</v>
       </c>
       <c r="G54" t="s">
-        <v>136</v>
+        <v>106</v>
       </c>
     </row>
     <row r="55" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F55" t="s">
-        <v>219</v>
+        <v>189</v>
       </c>
       <c r="G55" t="s">
-        <v>137</v>
+        <v>107</v>
       </c>
     </row>
     <row r="56" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F56" t="s">
-        <v>220</v>
+        <v>190</v>
       </c>
       <c r="G56" t="s">
-        <v>138</v>
+        <v>108</v>
       </c>
     </row>
     <row r="57" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F57" t="s">
-        <v>221</v>
+        <v>191</v>
       </c>
       <c r="G57" t="s">
-        <v>139</v>
+        <v>109</v>
       </c>
     </row>
     <row r="58" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F58" t="s">
-        <v>222</v>
+        <v>192</v>
       </c>
       <c r="G58" t="s">
-        <v>140</v>
+        <v>110</v>
       </c>
     </row>
     <row r="59" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F59" t="s">
-        <v>223</v>
+        <v>193</v>
       </c>
       <c r="G59" t="s">
-        <v>141</v>
+        <v>111</v>
       </c>
     </row>
     <row r="60" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F60" t="s">
-        <v>224</v>
+        <v>194</v>
       </c>
       <c r="G60" t="s">
-        <v>142</v>
+        <v>112</v>
       </c>
     </row>
     <row r="61" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F61" t="s">
-        <v>225</v>
+        <v>195</v>
       </c>
       <c r="G61" t="s">
-        <v>143</v>
+        <v>113</v>
       </c>
     </row>
     <row r="62" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F62" t="s">
-        <v>226</v>
+        <v>196</v>
       </c>
       <c r="G62" t="s">
-        <v>144</v>
+        <v>114</v>
       </c>
     </row>
     <row r="63" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F63" t="s">
-        <v>227</v>
+        <v>197</v>
       </c>
       <c r="G63" t="s">
-        <v>145</v>
+        <v>115</v>
       </c>
     </row>
     <row r="64" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F64" t="s">
-        <v>228</v>
+        <v>198</v>
       </c>
       <c r="G64" t="s">
-        <v>146</v>
+        <v>116</v>
       </c>
     </row>
     <row r="65" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F65" t="s">
-        <v>229</v>
+        <v>199</v>
       </c>
       <c r="G65" t="s">
-        <v>147</v>
+        <v>117</v>
       </c>
     </row>
     <row r="66" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F66" t="s">
-        <v>230</v>
+        <v>200</v>
       </c>
       <c r="G66" t="s">
-        <v>148</v>
+        <v>118</v>
       </c>
     </row>
     <row r="67" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F67" t="s">
-        <v>231</v>
+        <v>201</v>
       </c>
       <c r="G67" t="s">
-        <v>149</v>
+        <v>119</v>
       </c>
     </row>
     <row r="68" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F68" t="s">
-        <v>232</v>
+        <v>202</v>
       </c>
       <c r="G68" t="s">
-        <v>150</v>
+        <v>120</v>
       </c>
     </row>
     <row r="69" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F69" t="s">
-        <v>233</v>
+        <v>203</v>
       </c>
       <c r="G69" t="s">
-        <v>151</v>
+        <v>121</v>
       </c>
     </row>
     <row r="70" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F70" t="s">
-        <v>234</v>
+        <v>204</v>
       </c>
       <c r="G70" t="s">
-        <v>152</v>
+        <v>122</v>
       </c>
     </row>
     <row r="71" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F71" t="s">
-        <v>235</v>
+        <v>205</v>
       </c>
       <c r="G71" t="s">
-        <v>153</v>
+        <v>123</v>
       </c>
     </row>
     <row r="72" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F72" t="s">
-        <v>236</v>
+        <v>206</v>
       </c>
       <c r="G72" t="s">
-        <v>154</v>
+        <v>124</v>
       </c>
     </row>
     <row r="73" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F73" t="s">
-        <v>237</v>
+        <v>207</v>
       </c>
       <c r="G73" t="s">
-        <v>155</v>
+        <v>125</v>
       </c>
     </row>
     <row r="74" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F74" t="s">
-        <v>238</v>
+        <v>208</v>
       </c>
       <c r="G74" t="s">
-        <v>156</v>
+        <v>126</v>
       </c>
     </row>
     <row r="75" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F75" t="s">
-        <v>239</v>
+        <v>209</v>
       </c>
       <c r="G75" t="s">
-        <v>157</v>
+        <v>127</v>
       </c>
     </row>
     <row r="76" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F76" t="s">
-        <v>240</v>
+        <v>210</v>
       </c>
       <c r="G76" t="s">
-        <v>158</v>
+        <v>128</v>
       </c>
     </row>
     <row r="77" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F77" t="s">
-        <v>241</v>
+        <v>211</v>
       </c>
       <c r="G77" t="s">
-        <v>159</v>
+        <v>129</v>
       </c>
     </row>
     <row r="78" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F78" t="s">
-        <v>242</v>
+        <v>212</v>
       </c>
       <c r="G78" t="s">
-        <v>160</v>
+        <v>130</v>
       </c>
     </row>
     <row r="79" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F79" t="s">
-        <v>243</v>
+        <v>213</v>
       </c>
       <c r="G79" t="s">
-        <v>161</v>
+        <v>131</v>
       </c>
     </row>
     <row r="80" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F80" t="s">
-        <v>244</v>
+        <v>214</v>
       </c>
       <c r="G80" t="s">
-        <v>162</v>
+        <v>132</v>
       </c>
     </row>
     <row r="81" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F81" t="s">
-        <v>245</v>
+        <v>215</v>
       </c>
       <c r="G81" t="s">
-        <v>163</v>
+        <v>133</v>
       </c>
     </row>
     <row r="82" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F82" t="s">
-        <v>246</v>
+        <v>216</v>
       </c>
       <c r="G82" t="s">
-        <v>164</v>
+        <v>134</v>
       </c>
     </row>
     <row r="83" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F83" t="s">
-        <v>247</v>
+        <v>217</v>
       </c>
       <c r="G83" t="s">
-        <v>165</v>
+        <v>135</v>
       </c>
     </row>
     <row r="84" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F84" t="s">
-        <v>248</v>
+        <v>218</v>
       </c>
     </row>
     <row r="85" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F85" t="s">
-        <v>249</v>
+        <v>219</v>
       </c>
     </row>
     <row r="86" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F86" t="s">
-        <v>250</v>
+        <v>220</v>
       </c>
     </row>
     <row r="87" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F87" t="s">
-        <v>251</v>
+        <v>221</v>
       </c>
     </row>
     <row r="88" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F88" t="s">
-        <v>252</v>
+        <v>222</v>
       </c>
     </row>
     <row r="89" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F89" t="s">
-        <v>253</v>
+        <v>223</v>
       </c>
     </row>
     <row r="90" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F90" t="s">
-        <v>254</v>
+        <v>224</v>
       </c>
     </row>
     <row r="91" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F91" t="s">
-        <v>255</v>
+        <v>225</v>
       </c>
     </row>
     <row r="92" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F92" t="s">
-        <v>256</v>
+        <v>226</v>
       </c>
     </row>
     <row r="93" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F93" t="s">
-        <v>257</v>
+        <v>227</v>
       </c>
     </row>
     <row r="94" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F94" t="s">
-        <v>258</v>
+        <v>228</v>
       </c>
     </row>
     <row r="95" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F95" t="s">
-        <v>259</v>
+        <v>229</v>
       </c>
     </row>
     <row r="96" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F96" t="s">
-        <v>260</v>
+        <v>230</v>
       </c>
     </row>
     <row r="97" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F97" t="s">
-        <v>261</v>
+        <v>231</v>
       </c>
     </row>
     <row r="98" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F98" t="s">
-        <v>262</v>
+        <v>232</v>
       </c>
     </row>
     <row r="99" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F99" t="s">
-        <v>263</v>
+        <v>233</v>
       </c>
     </row>
     <row r="100" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F100" t="s">
-        <v>264</v>
+        <v>234</v>
       </c>
     </row>
     <row r="101" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F101" t="s">
-        <v>265</v>
+        <v>235</v>
       </c>
     </row>
     <row r="102" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F102" t="s">
-        <v>266</v>
+        <v>236</v>
       </c>
     </row>
     <row r="103" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F103" t="s">
-        <v>267</v>
+        <v>237</v>
       </c>
     </row>
     <row r="104" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F104" t="s">
-        <v>268</v>
+        <v>238</v>
       </c>
     </row>
     <row r="105" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F105" t="s">
-        <v>269</v>
+        <v>239</v>
       </c>
     </row>
     <row r="106" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F106" t="s">
-        <v>270</v>
+        <v>240</v>
       </c>
     </row>
     <row r="107" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F107" t="s">
-        <v>271</v>
+        <v>241</v>
       </c>
     </row>
     <row r="108" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F108" t="s">
-        <v>272</v>
+        <v>242</v>
       </c>
     </row>
   </sheetData>

</xml_diff>